<commit_message>
Brain: Completing the Acceptance Criteria for Continuous Integration Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A228900\Documents\Projects\continuum-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A228900\Documents\Projects\brain-edit\continuum-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="366">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1098,13 +1098,55 @@
   </si>
   <si>
     <t>Environments are provisioned on demand using automated tools like Chef. The teams can provision these environments and do not need to go through a rigorous process to obtain such environments. The team also has full access to such environments</t>
+  </si>
+  <si>
+    <t>The build and deployment processes are automated as much as the constraints allow. This should be automated preferably all the way to production, however, in some organisations this may not be possible. The steps to production exists and can be triggered manually on receiving the requisite approvals.</t>
+  </si>
+  <si>
+    <t>The team has a build pipeline that extends directly to production. Artefacts and code can be promoted through various environments all the way to production.</t>
+  </si>
+  <si>
+    <t>To speed up the regression tests feedback, the teams have parallelized the tests suites across multiple machines.</t>
+  </si>
+  <si>
+    <t>The team performs Continuous Integration in its truest form with short-lived branches and trunk-based development as the modus operandi. Branches are only used for exploration and short feature delivery but merged to the master branch and deleted as soon as the work is complete.</t>
+  </si>
+  <si>
+    <t>Team members check-in code multiple times each day. The check-ins have very small batches of changes and are very frequent usually having less than a few hours worth of work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All the environment and infrastructure specifications are treated similarly to code. They are managed and versioned and can be rebuilt from the version control management system entirely. </t>
+  </si>
+  <si>
+    <t>Team uses the build pipelines and continuous integration tools to provision infrastructure on demand. The team is able to provision and destroy environments without dependence on several external teams.</t>
+  </si>
+  <si>
+    <t>The release and change management process is catered for in the deployment process. Parts of the build pipeline address the governance around release and change management and the deployment process auto-generates the documentation required for the process.</t>
+  </si>
+  <si>
+    <t>As is required by continuous integration practices, the software product is always in a releasable state. The build pipeline is in a green (no failing tests/broken builds) state and every broken build state is fixed immediately or reverted to ensure that the application is in a releasable state always.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Release to the customers is a business decision rather than a technology decision. Business can trigger the release if they are happy with the functionality and technology is not a bottleneck for timeous customer releases. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The process is automated with business being able to release themselves should they want to.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1133,6 +1175,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1523,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3077,7 +3126,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>48</v>
       </c>
@@ -3090,12 +3139,14 @@
       <c r="D78" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E78" s="17"/>
+      <c r="E78" s="17" t="s">
+        <v>356</v>
+      </c>
       <c r="F78" s="9">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>48</v>
       </c>
@@ -3108,12 +3159,14 @@
       <c r="D79" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E79" s="17"/>
+      <c r="E79" s="17" t="s">
+        <v>357</v>
+      </c>
       <c r="F79" s="9">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>48</v>
       </c>
@@ -3126,12 +3179,14 @@
       <c r="D80" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E80" s="17"/>
+      <c r="E80" s="17" t="s">
+        <v>358</v>
+      </c>
       <c r="F80" s="14" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>48</v>
       </c>
@@ -3144,12 +3199,14 @@
       <c r="D81" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E81" s="17"/>
+      <c r="E81" s="17" t="s">
+        <v>359</v>
+      </c>
       <c r="F81" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>48</v>
       </c>
@@ -3162,12 +3219,14 @@
       <c r="D82" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E82" s="17"/>
+      <c r="E82" s="17" t="s">
+        <v>360</v>
+      </c>
       <c r="F82" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>48</v>
       </c>
@@ -3180,12 +3239,14 @@
       <c r="D83" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E83" s="17"/>
+      <c r="E83" s="17" t="s">
+        <v>361</v>
+      </c>
       <c r="F83" s="9">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>48</v>
       </c>
@@ -3198,12 +3259,14 @@
       <c r="D84" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="E84" s="17"/>
+      <c r="E84" s="17" t="s">
+        <v>362</v>
+      </c>
       <c r="F84" s="9">
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>48</v>
       </c>
@@ -3216,12 +3279,14 @@
       <c r="D85" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E85" s="17"/>
+      <c r="E85" s="17" t="s">
+        <v>363</v>
+      </c>
       <c r="F85" s="9">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>48</v>
       </c>
@@ -3234,12 +3299,14 @@
       <c r="D86" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E86" s="17"/>
+      <c r="E86" s="17" t="s">
+        <v>364</v>
+      </c>
       <c r="F86" s="9">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>48</v>
       </c>
@@ -3252,7 +3319,9 @@
       <c r="D87" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E87" s="17"/>
+      <c r="E87" s="17" t="s">
+        <v>365</v>
+      </c>
       <c r="F87" s="9">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Incident Management Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="383">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1140,6 +1140,57 @@
       </rPr>
       <t>The process is automated with business being able to release themselves should they want to.</t>
     </r>
+  </si>
+  <si>
+    <t>Current process for handling incidents is ad-hoc. The team needs to start instituting an incident management process and document it so it is easily accessible by all the team members.</t>
+  </si>
+  <si>
+    <t>An incident management process is documented and in place. The team knows where to find the document and uses it to manage incidents. Incidents are also recorded on the team wall.</t>
+  </si>
+  <si>
+    <t>There are key people identified to handle incidents and this is well known by the team.</t>
+  </si>
+  <si>
+    <t>There is very minimal handoffs. The resolution is effective and insolves very few teams, generally the core team and the dependent system team.</t>
+  </si>
+  <si>
+    <t>The incidents are recorded in the team backlog and prioritised together with all the other work in flight. There is an understanding of incident classification and the turn around time for the different classes of incidents. The team reacts appropriately based on the class of the incident.</t>
+  </si>
+  <si>
+    <t>Operational requirements for the application are identified and tracked in the backlog. Some of these requirements are MTTR, System Downtime, Service/Application response times, Service/Application downtime etc. These are displayed in dashboards in the team area.</t>
+  </si>
+  <si>
+    <t>The team is encouraged to address the root cause of the incidents/problems. The tasks are prioritised, estimated and planned within the iteration to give the team enough time to address the root cause.</t>
+  </si>
+  <si>
+    <t>Root cause analysis is performed for each incident.</t>
+  </si>
+  <si>
+    <t>The different support levels are in place and known by the team and stakeholders.</t>
+  </si>
+  <si>
+    <t>Team has implemented monitoring and alerting for the applications they are working on. This proactively lets the team know of any incidents before the stakeholders inform the team and the team strives to resolve incidents before they become evident to the stakeholders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defect management is automated and follows the same continuous integration life cycle as features. </t>
+  </si>
+  <si>
+    <t>For each defect, a test is written which is run on completion of the defect resolution as part of the regression suite to ensure that the defect does not re-occur or the team is notified if it re-occurs.</t>
+  </si>
+  <si>
+    <t>The system health is proactively monitored and displayed on dashboards in the team space. Some health status include MTTR, downtime, application response times, concurrent connections etc.</t>
+  </si>
+  <si>
+    <t>The root cause analysis tasks are tracked and recorded so the team has a history of them.</t>
+  </si>
+  <si>
+    <t>Each feature team does their own incident management as opposed to a centralised incident management team distributing tasks to the various teams.</t>
+  </si>
+  <si>
+    <t>The culture in the team is to fail forward. Incidents are managed, tracked and documented to ensure they are not repeated. Test cases are put in place to reduce the likelihood of failure.</t>
+  </si>
+  <si>
+    <t>The feature teams have dashboards monitoring the state of the application in production and uses the feedback from the monitoring to drive tasks for operational optimisation.</t>
   </si>
 </sst>
 </file>
@@ -1572,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3326,7 +3377,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>83</v>
       </c>
@@ -3339,12 +3390,14 @@
       <c r="D88" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E88" s="4"/>
+      <c r="E88" s="4" t="s">
+        <v>366</v>
+      </c>
       <c r="F88" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>83</v>
       </c>
@@ -3357,12 +3410,14 @@
       <c r="D89" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="E89" s="17"/>
+      <c r="E89" s="17" t="s">
+        <v>367</v>
+      </c>
       <c r="F89" s="9">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>83</v>
       </c>
@@ -3375,7 +3430,9 @@
       <c r="D90" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E90" s="17"/>
+      <c r="E90" s="17" t="s">
+        <v>368</v>
+      </c>
       <c r="F90" s="9">
         <v>87</v>
       </c>
@@ -3393,12 +3450,14 @@
       <c r="D91" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="E91" s="17"/>
+      <c r="E91" s="17" t="s">
+        <v>369</v>
+      </c>
       <c r="F91" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>83</v>
       </c>
@@ -3411,12 +3470,14 @@
       <c r="D92" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E92" s="17"/>
+      <c r="E92" s="17" t="s">
+        <v>370</v>
+      </c>
       <c r="F92" s="9">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
         <v>83</v>
       </c>
@@ -3429,12 +3490,14 @@
       <c r="D93" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E93" s="17"/>
+      <c r="E93" s="17" t="s">
+        <v>371</v>
+      </c>
       <c r="F93" s="9">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>83</v>
       </c>
@@ -3447,7 +3510,9 @@
       <c r="D94" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E94" s="17"/>
+      <c r="E94" s="17" t="s">
+        <v>372</v>
+      </c>
       <c r="F94" s="9">
         <v>0</v>
       </c>
@@ -3465,12 +3530,14 @@
       <c r="D95" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="E95" s="17"/>
+      <c r="E95" s="17" t="s">
+        <v>373</v>
+      </c>
       <c r="F95" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>83</v>
       </c>
@@ -3483,12 +3550,14 @@
       <c r="D96" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E96" s="17"/>
+      <c r="E96" s="17" t="s">
+        <v>374</v>
+      </c>
       <c r="F96" s="9">
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>83</v>
       </c>
@@ -3501,7 +3570,9 @@
       <c r="D97" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E97" s="17"/>
+      <c r="E97" s="17" t="s">
+        <v>375</v>
+      </c>
       <c r="F97" s="9">
         <v>0</v>
       </c>
@@ -3519,12 +3590,14 @@
       <c r="D98" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E98" s="17"/>
+      <c r="E98" s="17" t="s">
+        <v>376</v>
+      </c>
       <c r="F98" s="14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
         <v>83</v>
       </c>
@@ -3537,12 +3610,14 @@
       <c r="D99" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="E99" s="17"/>
+      <c r="E99" s="17" t="s">
+        <v>377</v>
+      </c>
       <c r="F99" s="14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>83</v>
       </c>
@@ -3555,12 +3630,14 @@
       <c r="D100" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="E100" s="17"/>
+      <c r="E100" s="17" t="s">
+        <v>378</v>
+      </c>
       <c r="F100" s="14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>83</v>
       </c>
@@ -3573,12 +3650,14 @@
       <c r="D101" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="E101" s="4"/>
+      <c r="E101" s="4" t="s">
+        <v>379</v>
+      </c>
       <c r="F101" s="14" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>83</v>
       </c>
@@ -3591,7 +3670,9 @@
       <c r="D102" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E102" s="17"/>
+      <c r="E102" s="17" t="s">
+        <v>380</v>
+      </c>
       <c r="F102" s="14" t="s">
         <v>265</v>
       </c>
@@ -3609,12 +3690,14 @@
       <c r="D103" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E103" s="17"/>
+      <c r="E103" s="17" t="s">
+        <v>381</v>
+      </c>
       <c r="F103" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>83</v>
       </c>
@@ -3627,7 +3710,9 @@
       <c r="D104" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E104" s="16"/>
+      <c r="E104" s="16" t="s">
+        <v>382</v>
+      </c>
       <c r="F104" s="14">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Risk Management Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="399">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1191,6 +1191,54 @@
   </si>
   <si>
     <t>The feature teams have dashboards monitoring the state of the application in production and uses the feedback from the monitoring to drive tasks for operational optimisation.</t>
+  </si>
+  <si>
+    <t>To be at this level, the team does not have a risk management process in place and simply does compliance with audits by ticking check boxes without necessarily implementing any processes to avert risk. To move from this level the team needs to start identifying, managing and tracking risk.</t>
+  </si>
+  <si>
+    <t>The team at this level is unable to clearly articulate what the risks are. The various risks are not transparent to the team and may be known by very few individuals within the team.</t>
+  </si>
+  <si>
+    <t>At this level, risks are captured by the team and tracked on the team wall and/or story management system. The team members can access the various risks and are all aware of what they are.</t>
+  </si>
+  <si>
+    <t>The risks are allocated owners as well as mititgation/action plans. These are clearly captured in the story management system.</t>
+  </si>
+  <si>
+    <t>The risks are discussed and reviewed as part of the iteration planning process and action items are allocated and assigned to prospective risk item owners. These are then tracked and reviewed throughout the iteration to ensure mitigation is in place.</t>
+  </si>
+  <si>
+    <t>Risks items are discussed during the agile ceremonies such as standups and they are updated accordingly to ensure they are not just recorded but are also mitigated. Any blockers are highlighted and addressed.</t>
+  </si>
+  <si>
+    <t>The team is able to identify/raise risks that do not have a mitigation plan and assign an owner, while recording on the wall.</t>
+  </si>
+  <si>
+    <t>All the risks have appropriate owners. Owners update during daily stand-ups on the progress towards mitigating the risks.</t>
+  </si>
+  <si>
+    <t>Cost benefit analysis of risk mitigations are discussed in the iteration planning sessions before risks are prioritised.</t>
+  </si>
+  <si>
+    <t>Roles, responsibilities and accountabilities for the risks owners are defined, agreed upon and documented where it is accessible by all team members.</t>
+  </si>
+  <si>
+    <t>There is clear communication with the business stakeholders and different stakeholders on the risks and mitigation plans in progress.</t>
+  </si>
+  <si>
+    <t>The team explicitly designs the risk mitigation and actions and are proactive rather than reactive towards the potential of risks.</t>
+  </si>
+  <si>
+    <t>Business stakeholders are also involved in the risks mitigation strategies and are aware of the effect of the various risks.</t>
+  </si>
+  <si>
+    <t>Risk management is used to identify potential opportunities and these are recorded in the story management system linking them to the risks. There is openess with respect to raising and highlighting risks and using them to inform the strategy.</t>
+  </si>
+  <si>
+    <t>The risks resolutions are measured and used to optimise the risk management process.</t>
+  </si>
+  <si>
+    <t>Financial impact of the risks are captured and availed to stakeholders and the team to drive more effective and optimised risk management.</t>
   </si>
 </sst>
 </file>
@@ -1623,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3717,7 +3765,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>90</v>
       </c>
@@ -3730,12 +3778,14 @@
       <c r="D105" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="E105" s="16"/>
+      <c r="E105" s="16" t="s">
+        <v>383</v>
+      </c>
       <c r="F105" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>90</v>
       </c>
@@ -3748,12 +3798,14 @@
       <c r="D106" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E106" s="16"/>
+      <c r="E106" s="16" t="s">
+        <v>384</v>
+      </c>
       <c r="F106" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>90</v>
       </c>
@@ -3766,12 +3818,14 @@
       <c r="D107" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E107" s="16"/>
+      <c r="E107" s="16" t="s">
+        <v>385</v>
+      </c>
       <c r="F107" s="14">
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>90</v>
       </c>
@@ -3784,12 +3838,14 @@
       <c r="D108" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="E108" s="17"/>
+      <c r="E108" s="17" t="s">
+        <v>386</v>
+      </c>
       <c r="F108" s="14">
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>90</v>
       </c>
@@ -3802,7 +3858,9 @@
       <c r="D109" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="E109" s="17"/>
+      <c r="E109" s="17" t="s">
+        <v>387</v>
+      </c>
       <c r="F109" s="14">
         <v>105</v>
       </c>
@@ -3820,12 +3878,14 @@
       <c r="D110" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E110" s="16"/>
+      <c r="E110" s="16" t="s">
+        <v>388</v>
+      </c>
       <c r="F110" s="14">
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>90</v>
       </c>
@@ -3838,7 +3898,9 @@
       <c r="D111" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E111" s="16"/>
+      <c r="E111" s="16" t="s">
+        <v>389</v>
+      </c>
       <c r="F111" s="19">
         <v>107108</v>
       </c>
@@ -3856,7 +3918,9 @@
       <c r="D112" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E112" s="17"/>
+      <c r="E112" s="17" t="s">
+        <v>390</v>
+      </c>
       <c r="F112" s="14">
         <v>0</v>
       </c>
@@ -3874,12 +3938,14 @@
       <c r="D113" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="E113" s="17"/>
+      <c r="E113" s="17" t="s">
+        <v>391</v>
+      </c>
       <c r="F113" s="14">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>90</v>
       </c>
@@ -3892,7 +3958,9 @@
       <c r="D114" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="E114" s="17"/>
+      <c r="E114" s="17" t="s">
+        <v>392</v>
+      </c>
       <c r="F114" s="14">
         <v>111</v>
       </c>
@@ -3910,7 +3978,9 @@
       <c r="D115" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E115" s="17"/>
+      <c r="E115" s="17" t="s">
+        <v>393</v>
+      </c>
       <c r="F115" s="14">
         <v>0</v>
       </c>
@@ -3928,12 +3998,14 @@
       <c r="D116" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E116" s="17"/>
+      <c r="E116" s="17" t="s">
+        <v>394</v>
+      </c>
       <c r="F116" s="14">
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>90</v>
       </c>
@@ -3946,12 +4018,14 @@
       <c r="D117" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E117" s="17"/>
+      <c r="E117" s="17" t="s">
+        <v>395</v>
+      </c>
       <c r="F117" s="14">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>90</v>
       </c>
@@ -3964,7 +4038,9 @@
       <c r="D118" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E118" s="17"/>
+      <c r="E118" s="17" t="s">
+        <v>396</v>
+      </c>
       <c r="F118" s="14">
         <v>0</v>
       </c>
@@ -3982,12 +4058,14 @@
       <c r="D119" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E119" s="17"/>
+      <c r="E119" s="17" t="s">
+        <v>397</v>
+      </c>
       <c r="F119" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>90</v>
       </c>
@@ -4000,7 +4078,9 @@
       <c r="D120" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E120" s="17"/>
+      <c r="E120" s="17" t="s">
+        <v>398</v>
+      </c>
       <c r="F120" s="14">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Software Design Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="415">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1239,6 +1239,54 @@
   </si>
   <si>
     <t>Financial impact of the risks are captured and availed to stakeholders and the team to drive more effective and optimised risk management.</t>
+  </si>
+  <si>
+    <t>Design and technical decisions are done in an adhoc manner with no vision of the application road map. Technical team members are not aware of the overall technical design decisions and this is not documented in any form.</t>
+  </si>
+  <si>
+    <t>At this level of proficiency, the team does a lot of Big Up-Front designs for the systems as opposed to a just enough design approach. There are several ceremonial design sessions for the entire application without necessarily taken into effect the fact that there might need to be changes should the product vision change.</t>
+  </si>
+  <si>
+    <t>Technologists at this level of proficiency design highly tightly coupled and brittle systems. The goal should be to start designing loosely coupled systems so that they are independently deployable and can be monitored in isolation.</t>
+  </si>
+  <si>
+    <t>At this proficiency level, the designs are done more regularly and reviews are put in place to ensure that product vision change causes a validation of the technical design. The team also gets a view of the technical design decisions and roadmap.</t>
+  </si>
+  <si>
+    <t>Design assumptions are tracked and recorded on the team wall and these are validated during the iteration as well as during the iteration planning sessions.</t>
+  </si>
+  <si>
+    <t>Design issues identified are tracked and prioritised in the backlog and attended to similar to the technical debts.</t>
+  </si>
+  <si>
+    <t>The system non-functional requirements are documented and tracked. These are also prioritised in the backlog.</t>
+  </si>
+  <si>
+    <t>The team emphasizes a modular design of the application with clearly defined interfaces between the modules and clear communication protocols between the modules (for example clearly defined APIs using RESTful protocols).</t>
+  </si>
+  <si>
+    <t>The technical design is owned by the feature teams. The technical architect is part of the core team and is not a stakeholder external to the team making decisions on their behalf.</t>
+  </si>
+  <si>
+    <t>Some design decisions can be linked to the requirements, however, not all the design decisions are.</t>
+  </si>
+  <si>
+    <t>The design requirements are captured in automated test cases, to ensure that these have been met.</t>
+  </si>
+  <si>
+    <t>Non-functional requirements are clearly defined and documented. Associated metrics are tracked on the team dashboards automatically and are constantly monitored and optimized.</t>
+  </si>
+  <si>
+    <t>Modules of the system can be simulated using stubs or mocks where applicable to ensure autonomy and isolation.</t>
+  </si>
+  <si>
+    <t>Design is captured in a model and generated by software applications.</t>
+  </si>
+  <si>
+    <t>All the design decisions can be traced to system requirements.</t>
+  </si>
+  <si>
+    <t>Design happens as a Just-In-Time activity following paradigms like TDD and Evolutionary Architecture.</t>
   </si>
 </sst>
 </file>
@@ -1671,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4085,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>102</v>
       </c>
@@ -4098,12 +4146,14 @@
       <c r="D121" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E121" s="17"/>
+      <c r="E121" s="17" t="s">
+        <v>399</v>
+      </c>
       <c r="F121" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>102</v>
       </c>
@@ -4116,12 +4166,14 @@
       <c r="D122" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E122" s="17"/>
+      <c r="E122" s="17" t="s">
+        <v>400</v>
+      </c>
       <c r="F122" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>102</v>
       </c>
@@ -4134,12 +4186,14 @@
       <c r="D123" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E123" s="4"/>
+      <c r="E123" s="4" t="s">
+        <v>401</v>
+      </c>
       <c r="F123" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>102</v>
       </c>
@@ -4152,12 +4206,14 @@
       <c r="D124" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E124" s="17"/>
+      <c r="E124" s="17" t="s">
+        <v>402</v>
+      </c>
       <c r="F124" s="14">
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>102</v>
       </c>
@@ -4170,12 +4226,14 @@
       <c r="D125" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E125" s="4"/>
+      <c r="E125" s="4" t="s">
+        <v>403</v>
+      </c>
       <c r="F125" s="14">
         <v>121</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>102</v>
       </c>
@@ -4188,12 +4246,14 @@
       <c r="D126" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E126" s="17"/>
+      <c r="E126" s="17" t="s">
+        <v>404</v>
+      </c>
       <c r="F126" s="14">
         <v>123</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>102</v>
       </c>
@@ -4206,12 +4266,14 @@
       <c r="D127" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E127" s="17"/>
+      <c r="E127" s="17" t="s">
+        <v>405</v>
+      </c>
       <c r="F127" s="14">
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>102</v>
       </c>
@@ -4224,12 +4286,14 @@
       <c r="D128" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="E128" s="17"/>
+      <c r="E128" s="17" t="s">
+        <v>406</v>
+      </c>
       <c r="F128" s="14">
         <v>122</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
         <v>102</v>
       </c>
@@ -4242,12 +4306,14 @@
       <c r="D129" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="E129" s="17"/>
+      <c r="E129" s="17" t="s">
+        <v>407</v>
+      </c>
       <c r="F129" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>102</v>
       </c>
@@ -4260,12 +4326,14 @@
       <c r="D130" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="E130" s="17"/>
+      <c r="E130" s="17" t="s">
+        <v>408</v>
+      </c>
       <c r="F130" s="14">
         <v>125</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>102</v>
       </c>
@@ -4278,12 +4346,14 @@
       <c r="D131" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="E131" s="17"/>
+      <c r="E131" s="17" t="s">
+        <v>409</v>
+      </c>
       <c r="F131" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>102</v>
       </c>
@@ -4296,12 +4366,14 @@
       <c r="D132" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E132" s="17"/>
+      <c r="E132" s="17" t="s">
+        <v>410</v>
+      </c>
       <c r="F132" s="14">
         <v>126</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>102</v>
       </c>
@@ -4314,7 +4386,9 @@
       <c r="D133" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E133" s="17"/>
+      <c r="E133" s="17" t="s">
+        <v>411</v>
+      </c>
       <c r="F133" s="14">
         <v>127</v>
       </c>
@@ -4332,7 +4406,9 @@
       <c r="D134" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E134" s="17"/>
+      <c r="E134" s="17" t="s">
+        <v>412</v>
+      </c>
       <c r="F134" s="14">
         <v>0</v>
       </c>
@@ -4350,12 +4426,14 @@
       <c r="D135" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="E135" s="17"/>
+      <c r="E135" s="17" t="s">
+        <v>413</v>
+      </c>
       <c r="F135" s="14">
         <v>129</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>102</v>
       </c>
@@ -4368,7 +4446,9 @@
       <c r="D136" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E136" s="17"/>
+      <c r="E136" s="17" t="s">
+        <v>414</v>
+      </c>
       <c r="F136" s="14">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Teaming Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="429">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1287,6 +1287,48 @@
   </si>
   <si>
     <t>Design happens as a Just-In-Time activity following paradigms like TDD and Evolutionary Architecture.</t>
+  </si>
+  <si>
+    <t>The teams at this level of proficiency do not have autonomy with respect to decision making. They need to consult for any decisions they make and cannot be qualified as autonomous teams. To move from this level teams need to start making their own decisions and have some autonomy.</t>
+  </si>
+  <si>
+    <t>The teams work of functionality without necessarily knowing what the goal and vision is. Some people in the team or some stakeholders may know the vision but this is not shared across and this has not been documented. The goals/vision need to be documented and easily accessible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Few individuals in the team understand the stakeholder landscape but the whole team is unaware of the entire stakeholder landscape. </t>
+  </si>
+  <si>
+    <t>Team works towards shared goals and vision which is agreed, captured and understood. The vision is clear on the team wall and also recorded on the story management system.</t>
+  </si>
+  <si>
+    <t>The teams steakholders are clearly understood and also captured on the team story management system. This is accessible to all team members.</t>
+  </si>
+  <si>
+    <t>The definition of "done" is well understood by the team and this is also captured on the team wall.</t>
+  </si>
+  <si>
+    <t>The team is always actively seeking feedback from stakeholders and action items are captured and prioritised towards achieving the team goals.</t>
+  </si>
+  <si>
+    <t>There is a high level of collective ownership and collaboration within the team</t>
+  </si>
+  <si>
+    <t>The blockers and dependencies are minimised and managed. These are recorded on the story management system and captured on the team walls making them very visible to all the team members.</t>
+  </si>
+  <si>
+    <t>There is open communication lines in the team and all members are able to contribute as appropriate. Retrospectives are used to elicit participation from every member in the team.</t>
+  </si>
+  <si>
+    <t>The team has measures in place to monitor success and this is visually communicated to the team members and the stakeholders.</t>
+  </si>
+  <si>
+    <t>The team is completely autonomous and drives all decision making. Consultations are used to get information that can feed into their decision making but the decision making is entirely up to the teams.</t>
+  </si>
+  <si>
+    <t>Team collectively acknowledges failure or success and the culture is driven by collective ownership.</t>
+  </si>
+  <si>
+    <t>Retrospectives happen every iteration. Action items from retrospectives are tracked and used to drive continuous improvement.</t>
   </si>
 </sst>
 </file>
@@ -1719,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4453,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
         <v>115</v>
       </c>
@@ -4466,12 +4508,14 @@
       <c r="D137" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="E137" s="17"/>
+      <c r="E137" s="17" t="s">
+        <v>415</v>
+      </c>
       <c r="F137" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
         <v>115</v>
       </c>
@@ -4484,12 +4528,14 @@
       <c r="D138" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="E138" s="17"/>
+      <c r="E138" s="17" t="s">
+        <v>416</v>
+      </c>
       <c r="F138" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
         <v>115</v>
       </c>
@@ -4502,12 +4548,14 @@
       <c r="D139" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="E139" s="17"/>
+      <c r="E139" s="17" t="s">
+        <v>417</v>
+      </c>
       <c r="F139" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
         <v>115</v>
       </c>
@@ -4520,7 +4568,9 @@
       <c r="D140" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E140" s="17"/>
+      <c r="E140" s="17" t="s">
+        <v>418</v>
+      </c>
       <c r="F140" s="14">
         <v>137</v>
       </c>
@@ -4538,7 +4588,9 @@
       <c r="D141" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="E141" s="17"/>
+      <c r="E141" s="17" t="s">
+        <v>419</v>
+      </c>
       <c r="F141" s="14">
         <v>138</v>
       </c>
@@ -4556,12 +4608,14 @@
       <c r="D142" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="E142" s="17"/>
+      <c r="E142" s="17" t="s">
+        <v>420</v>
+      </c>
       <c r="F142" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>115</v>
       </c>
@@ -4574,12 +4628,14 @@
       <c r="D143" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="E143" s="17"/>
+      <c r="E143" s="17" t="s">
+        <v>421</v>
+      </c>
       <c r="F143" s="14">
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>115</v>
       </c>
@@ -4592,12 +4648,14 @@
       <c r="D144" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="E144" s="17"/>
+      <c r="E144" s="17" t="s">
+        <v>422</v>
+      </c>
       <c r="F144" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
         <v>115</v>
       </c>
@@ -4610,12 +4668,14 @@
       <c r="D145" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="E145" s="17"/>
+      <c r="E145" s="17" t="s">
+        <v>423</v>
+      </c>
       <c r="F145" s="14">
         <v>141</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
         <v>115</v>
       </c>
@@ -4628,12 +4688,14 @@
       <c r="D146" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E146" s="17"/>
+      <c r="E146" s="17" t="s">
+        <v>424</v>
+      </c>
       <c r="F146" s="14">
         <v>143</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
         <v>115</v>
       </c>
@@ -4646,12 +4708,14 @@
       <c r="D147" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E147" s="17"/>
+      <c r="E147" s="17" t="s">
+        <v>425</v>
+      </c>
       <c r="F147" s="14">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
         <v>115</v>
       </c>
@@ -4664,7 +4728,9 @@
       <c r="D148" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E148" s="17"/>
+      <c r="E148" s="17" t="s">
+        <v>426</v>
+      </c>
       <c r="F148" s="14">
         <v>136</v>
       </c>
@@ -4682,12 +4748,14 @@
       <c r="D149" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="E149" s="17"/>
+      <c r="E149" s="17" t="s">
+        <v>427</v>
+      </c>
       <c r="F149" s="14">
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>115</v>
       </c>
@@ -4700,7 +4768,9 @@
       <c r="D150" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E150" s="17"/>
+      <c r="E150" s="17" t="s">
+        <v>428</v>
+      </c>
       <c r="F150" s="14">
         <v>147</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Release Management Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="449">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1329,6 +1329,66 @@
   </si>
   <si>
     <t>Retrospectives happen every iteration. Action items from retrospectives are tracked and used to drive continuous improvement.</t>
+  </si>
+  <si>
+    <t>The release cycle is extremely long. It takes 6months or more to release software into production. The team needs to work on reducing the cycle time</t>
+  </si>
+  <si>
+    <t>Deployment is manual and very complex. It is generally a ceremony which requires high coordination between several stakeholders such as DBAs, Ops, Devs etc. This needs to be optimized and simplified so that the team is responsible for the deployment. Manual interventions should be minimized.</t>
+  </si>
+  <si>
+    <t>The pace and delivery of work is inconsistent. The team is unable to give a definitive answer on when features will be delivered in production or how long it will take for the team to avail a certain feature to the customers upon completion of the development tasks.</t>
+  </si>
+  <si>
+    <t>Each environment has it's own artefacts with high levels of configuration required to make them work in those environments. The team needs to start moving towards a configuration-as-code approach where the artefacts can simply be promoted from one environment to the other painlessly.</t>
+  </si>
+  <si>
+    <t>The team is able to plan releases to a regular cycle and can track and manage features within regular time frames. Delivery is more predictable and captured on the team walls.</t>
+  </si>
+  <si>
+    <t>The release dates are seldom moved out. The team is able to rather reduce the release features rather than the move out the release dates.</t>
+  </si>
+  <si>
+    <t>There is a well defined process for handling the release of the artefacts to operations and support teams in places. This is documented and well understood by all the team members. The team at this level is investigating means of embedding operations/support in the team structure.</t>
+  </si>
+  <si>
+    <t>Build artefacts are well defined and produced preferably by the build/continuous integration tool. These artefacts are readily available to the team as well as the operations and support teams. The team is able to tell which artefact was deployed when.</t>
+  </si>
+  <si>
+    <t>The releases and deployments are automated using pipelines. These pipelines are visible on dashboards in the team spaces. There may however still be some manual dependencies such as environment configurations but the artefacts are packaged in a ready to deploy state.</t>
+  </si>
+  <si>
+    <t>Teams have a high level of confidence for releases. Releases are no longer considered as a ceremonial activity but as a regular cadence.</t>
+  </si>
+  <si>
+    <t>Release notes are automatically generated as part of the release/build scripts.</t>
+  </si>
+  <si>
+    <t>The team does not have a key man dependency for releases. The release process is automated such that any individual in the team can perform a release. Releases can be audited and tracked.</t>
+  </si>
+  <si>
+    <t>The operations teams collaborate very closely with the delivery teams and have backlog item tasks during development of the features to ensure that on completing development the applications are also ready to be deployed and released.</t>
+  </si>
+  <si>
+    <t>The team constantly tracks and monitors the release metrics and trends on the story wall and all stakeholders are able to interact with these metrics on the dashboards.</t>
+  </si>
+  <si>
+    <t>Releases can be deployed at anytime due to complete automation of the release tasks. Teams have release scripts and these are integrated in the build pipelines and dashboards.</t>
+  </si>
+  <si>
+    <t>The team controls the release and does not depend on a third party team to compile and release their software. They can release software anytime to any of the environments.</t>
+  </si>
+  <si>
+    <t>The product owner can decide when the release goes into production. In certain instances, the product owner can click on the deploy to production button and trigger a release to production.</t>
+  </si>
+  <si>
+    <t>The operations team is part of the product/program team as opposed to being a hand-off team. They work hand-in-hand with the development teams to ensure the readiness of the application for production releases.</t>
+  </si>
+  <si>
+    <t>Releases happen frequently and are routine. There are no application roll backs but rather roll forwards. Redeployment is favoured over system roll backs.</t>
+  </si>
+  <si>
+    <t>Team is able to release toggled off features using methodologies like Feature Toggling or Branching by Abstraction. Team is able to perform Blue-Green deployments with minimal downtimes to the application from a customer perspective.</t>
   </si>
 </sst>
 </file>
@@ -1761,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E151" sqref="E151"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4775,7 +4835,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A151" s="6" t="s">
         <v>122</v>
       </c>
@@ -4788,12 +4848,14 @@
       <c r="D151" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E151" s="17"/>
+      <c r="E151" s="17" t="s">
+        <v>429</v>
+      </c>
       <c r="F151" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>122</v>
       </c>
@@ -4806,12 +4868,14 @@
       <c r="D152" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="E152" s="17"/>
+      <c r="E152" s="17" t="s">
+        <v>430</v>
+      </c>
       <c r="F152" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
         <v>122</v>
       </c>
@@ -4824,12 +4888,14 @@
       <c r="D153" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E153" s="17"/>
+      <c r="E153" s="17" t="s">
+        <v>431</v>
+      </c>
       <c r="F153" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
         <v>122</v>
       </c>
@@ -4842,12 +4908,14 @@
       <c r="D154" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="E154" s="17"/>
+      <c r="E154" s="17" t="s">
+        <v>432</v>
+      </c>
       <c r="F154" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
         <v>122</v>
       </c>
@@ -4860,12 +4928,14 @@
       <c r="D155" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="E155" s="17"/>
+      <c r="E155" s="17" t="s">
+        <v>433</v>
+      </c>
       <c r="F155" s="14">
         <v>151</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
         <v>122</v>
       </c>
@@ -4878,12 +4948,14 @@
       <c r="D156" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="E156" s="17"/>
+      <c r="E156" s="17" t="s">
+        <v>434</v>
+      </c>
       <c r="F156" s="14">
         <v>152</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>122</v>
       </c>
@@ -4896,12 +4968,14 @@
       <c r="D157" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="E157" s="17"/>
+      <c r="E157" s="17" t="s">
+        <v>435</v>
+      </c>
       <c r="F157" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>122</v>
       </c>
@@ -4914,12 +4988,14 @@
       <c r="D158" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="E158" s="17"/>
+      <c r="E158" s="17" t="s">
+        <v>436</v>
+      </c>
       <c r="F158" s="14">
         <v>154</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>122</v>
       </c>
@@ -4932,12 +5008,14 @@
       <c r="D159" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="E159" s="17"/>
+      <c r="E159" s="17" t="s">
+        <v>437</v>
+      </c>
       <c r="F159" s="14">
         <v>155</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>122</v>
       </c>
@@ -4950,12 +5028,14 @@
       <c r="D160" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="E160" s="17"/>
+      <c r="E160" s="17" t="s">
+        <v>438</v>
+      </c>
       <c r="F160" s="19">
         <v>156157</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
         <v>122</v>
       </c>
@@ -4968,12 +5048,14 @@
       <c r="D161" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E161" s="17"/>
+      <c r="E161" s="17" t="s">
+        <v>439</v>
+      </c>
       <c r="F161" s="14">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
         <v>122</v>
       </c>
@@ -4986,12 +5068,14 @@
       <c r="D162" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="E162" s="17"/>
+      <c r="E162" s="17" t="s">
+        <v>440</v>
+      </c>
       <c r="F162" s="14">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
         <v>122</v>
       </c>
@@ -5004,12 +5088,14 @@
       <c r="D163" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="E163" s="17"/>
+      <c r="E163" s="17" t="s">
+        <v>441</v>
+      </c>
       <c r="F163" s="14">
         <v>160</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
         <v>122</v>
       </c>
@@ -5022,12 +5108,14 @@
       <c r="D164" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="E164" s="17"/>
+      <c r="E164" s="17" t="s">
+        <v>442</v>
+      </c>
       <c r="F164" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
         <v>122</v>
       </c>
@@ -5040,12 +5128,14 @@
       <c r="D165" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="E165" s="17"/>
+      <c r="E165" s="17" t="s">
+        <v>443</v>
+      </c>
       <c r="F165" s="19">
         <v>161</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
         <v>122</v>
       </c>
@@ -5058,12 +5148,14 @@
       <c r="D166" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="E166" s="17"/>
+      <c r="E166" s="17" t="s">
+        <v>444</v>
+      </c>
       <c r="F166" s="19">
         <v>162</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>122</v>
       </c>
@@ -5076,12 +5168,14 @@
       <c r="D167" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="E167" s="17"/>
+      <c r="E167" s="17" t="s">
+        <v>445</v>
+      </c>
       <c r="F167" s="19">
         <v>161</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>122</v>
       </c>
@@ -5094,7 +5188,9 @@
       <c r="D168" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="E168" s="17"/>
+      <c r="E168" s="17" t="s">
+        <v>446</v>
+      </c>
       <c r="F168" s="14">
         <v>163</v>
       </c>
@@ -5112,12 +5208,14 @@
       <c r="D169" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="E169" s="17"/>
+      <c r="E169" s="17" t="s">
+        <v>447</v>
+      </c>
       <c r="F169" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
         <v>122</v>
       </c>
@@ -5130,7 +5228,9 @@
       <c r="D170" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="E170" s="17"/>
+      <c r="E170" s="17" t="s">
+        <v>448</v>
+      </c>
       <c r="F170" s="14">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Quality Assurance Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="475">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1389,6 +1389,84 @@
   </si>
   <si>
     <t>Team is able to release toggled off features using methodologies like Feature Toggling or Branching by Abstraction. Team is able to perform Blue-Green deployments with minimal downtimes to the application from a customer perspective.</t>
+  </si>
+  <si>
+    <t>The testing is purely manual at this level of maturity. Teams rely on manual testers to find defects and bugs. Teams need to start writing some automated tests</t>
+  </si>
+  <si>
+    <t>The cycle time of features and functionality is impacted due to testing late in the lifecycle. Functionality is stopped from being deployed due to defects/bugs being found at later stages of the lifecycle.</t>
+  </si>
+  <si>
+    <t>Non-functional testing is considered as an afterthought when the Software is about to be released. Teams do not factor non-functional testing in their designs and implementation. Teams need to start considering non-functional testing such as how the application will behave under load into consideration.</t>
+  </si>
+  <si>
+    <t>There is a separate testing team that designs test cases based on the requirements document without interacting with the teams. There should be closer collaboration with the development team.</t>
+  </si>
+  <si>
+    <t>The code base has very little or no unit/integration tests. Developers rely on testers to find bugs/defects in their implementation.</t>
+  </si>
+  <si>
+    <t>The Quality Assurance assets are non-reusable due to it being very manual and specific to each application. The test cases are driven by the requirements so no frameworks in place. The team should start investigating frameworks, which can be extended for other test cases so that any team member is able to contribute to testing.</t>
+  </si>
+  <si>
+    <t>At this maturity level, some of the regression tests are automated eventhough all the business critical cases do not have automated regression tests.</t>
+  </si>
+  <si>
+    <t>The regression tests are run on an ad hoc basis as opposed to on every critical change to the application. The regression tests should be run as part of the build and release towards production automatically to move from this level</t>
+  </si>
+  <si>
+    <t>The test cases are designed by the team working on the application in collaboration with the stake holders. The team is aware of the business critical functionality and designs test cases to cater for these.</t>
+  </si>
+  <si>
+    <t>Regression test packs are fully automated for the application.</t>
+  </si>
+  <si>
+    <t>Regression tests are triggered by the build pipeline and run as part of the normal pipeline process. They are scheduled as daily run tasks due to the typical slowness in regression tests execution.</t>
+  </si>
+  <si>
+    <t>The team has implemented smoke tests and these are run as part of every code check-in. The smoke tests report are also displayed on the team tests metrics on the dashboard.</t>
+  </si>
+  <si>
+    <t>Performance tests are automated and the performance metrics are displayed on the dashboards. The build pipeline is failed if the performance metrics expected is not met. Due to the slow nature of performance tests, these are run as scheduled tasks on a nightly basis.</t>
+  </si>
+  <si>
+    <t>Non-functional requirements such as response times are defined and measured with test cases that are also displayed on the dashboards.</t>
+  </si>
+  <si>
+    <t>The team designs the test cases as part of the iteration and when building the functionality as opposed to as a pre-project process. Test cases are adapted to suit changes in the product vision and goal.</t>
+  </si>
+  <si>
+    <t>Infrastructure is automated and can be generated from scripts in the version control management system. The infrastructure automation is also tested using tools like ChefSpec.</t>
+  </si>
+  <si>
+    <t>Automation security testing is implemented and is part of the build pipeline using tools such as ZAP (Zed-Attack Proxy). The build is failed if security testing fails.</t>
+  </si>
+  <si>
+    <t>Test are automated and only the exploratory type tests are left unautomated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quality metrics are measured and tracked. Historical trends of the quality metrics are displayed on dashboards to the teams to drive the right culture of always improving quality. </t>
+  </si>
+  <si>
+    <t>The team writes unit tests using established frameworks and methodologies. The unit tests coverage is not less than 50% and the build is failed if the unit tests coverage is lower than this. Developers write tests as they build functionality. Testing is not out-sourced to quality assurance engineers.</t>
+  </si>
+  <si>
+    <t>Any team member can execute the tests via script runs or on the build pipelines.</t>
+  </si>
+  <si>
+    <t>There are documented processes in place to understand the root cause of test failures and how to respond to them especially for the non-functional requirements testing.</t>
+  </si>
+  <si>
+    <t>Tests artefacts have same significance and importance as the application code and are continually refactored and maintained.</t>
+  </si>
+  <si>
+    <t>At least 50% of the code base is test covered. The test coverage metrics are captured on the team pipeline dashboards and the build is failed if the coverage threshold is less than 50%. A failing tests is always fixed before extra functionality is built.</t>
+  </si>
+  <si>
+    <t>Performance metrics are clearly defined and available to the team members early in the lifecycle. These are displayed on the team walls for all team members to be aware of and reviewed every iteration.</t>
+  </si>
+  <si>
+    <t>Tests drive the release readiness while business drives the release decisions. A release candidate is only generated and available in the pipeline if all the tests have passed.</t>
   </si>
 </sst>
 </file>
@@ -1821,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E171" sqref="E171"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E197" sqref="E197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5235,7 +5313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
         <v>134</v>
       </c>
@@ -5248,12 +5326,14 @@
       <c r="D171" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E171" s="17"/>
+      <c r="E171" s="17" t="s">
+        <v>449</v>
+      </c>
       <c r="F171" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
         <v>134</v>
       </c>
@@ -5266,12 +5346,14 @@
       <c r="D172" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E172" s="17"/>
+      <c r="E172" s="17" t="s">
+        <v>450</v>
+      </c>
       <c r="F172" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>134</v>
       </c>
@@ -5284,12 +5366,14 @@
       <c r="D173" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E173" s="17"/>
+      <c r="E173" s="17" t="s">
+        <v>451</v>
+      </c>
       <c r="F173" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>134</v>
       </c>
@@ -5302,12 +5386,14 @@
       <c r="D174" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="E174" s="17"/>
+      <c r="E174" s="17" t="s">
+        <v>452</v>
+      </c>
       <c r="F174" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>134</v>
       </c>
@@ -5320,12 +5406,14 @@
       <c r="D175" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E175" s="16"/>
+      <c r="E175" s="16" t="s">
+        <v>453</v>
+      </c>
       <c r="F175" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>134</v>
       </c>
@@ -5338,12 +5426,14 @@
       <c r="D176" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E176" s="3"/>
+      <c r="E176" s="3" t="s">
+        <v>454</v>
+      </c>
       <c r="F176" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
         <v>134</v>
       </c>
@@ -5356,12 +5446,14 @@
       <c r="D177" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E177" s="16"/>
+      <c r="E177" s="16" t="s">
+        <v>455</v>
+      </c>
       <c r="F177" s="19">
         <v>171172173</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
         <v>134</v>
       </c>
@@ -5374,12 +5466,14 @@
       <c r="D178" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="E178" s="16"/>
+      <c r="E178" s="16" t="s">
+        <v>456</v>
+      </c>
       <c r="F178" s="19">
         <v>171172173</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
         <v>134</v>
       </c>
@@ -5392,7 +5486,9 @@
       <c r="D179" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E179" s="16"/>
+      <c r="E179" s="16" t="s">
+        <v>457</v>
+      </c>
       <c r="F179" s="14">
         <v>174</v>
       </c>
@@ -5410,12 +5506,14 @@
       <c r="D180" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E180" s="16"/>
+      <c r="E180" s="16" t="s">
+        <v>458</v>
+      </c>
       <c r="F180" s="19">
         <v>177178</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
         <v>134</v>
       </c>
@@ -5428,12 +5526,14 @@
       <c r="D181" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="E181" s="16"/>
+      <c r="E181" s="16" t="s">
+        <v>459</v>
+      </c>
       <c r="F181" s="19">
         <v>177178</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
         <v>134</v>
       </c>
@@ -5446,12 +5546,14 @@
       <c r="D182" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E182" s="16"/>
+      <c r="E182" s="16" t="s">
+        <v>472</v>
+      </c>
       <c r="F182" s="19">
         <v>177178</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>134</v>
       </c>
@@ -5464,12 +5566,14 @@
       <c r="D183" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="E183" s="16"/>
+      <c r="E183" s="16" t="s">
+        <v>460</v>
+      </c>
       <c r="F183" s="19">
         <v>177178</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
         <v>134</v>
       </c>
@@ -5482,12 +5586,14 @@
       <c r="D184" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E184" s="16"/>
+      <c r="E184" s="16" t="s">
+        <v>461</v>
+      </c>
       <c r="F184" s="19">
         <v>177178</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
         <v>134</v>
       </c>
@@ -5500,12 +5606,14 @@
       <c r="D185" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E185" s="16"/>
+      <c r="E185" s="16" t="s">
+        <v>462</v>
+      </c>
       <c r="F185" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
         <v>134</v>
       </c>
@@ -5518,12 +5626,14 @@
       <c r="D186" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E186" s="16"/>
+      <c r="E186" s="16" t="s">
+        <v>463</v>
+      </c>
       <c r="F186" s="14">
         <v>179</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A187" s="6" t="s">
         <v>134</v>
       </c>
@@ -5536,12 +5646,14 @@
       <c r="D187" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E187" s="16"/>
+      <c r="E187" s="16" t="s">
+        <v>468</v>
+      </c>
       <c r="F187" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
         <v>134</v>
       </c>
@@ -5554,12 +5666,14 @@
       <c r="D188" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E188" s="16"/>
+      <c r="E188" s="16" t="s">
+        <v>464</v>
+      </c>
       <c r="F188" s="19">
         <v>180181182183184</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
         <v>134</v>
       </c>
@@ -5572,12 +5686,14 @@
       <c r="D189" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="E189" s="16"/>
+      <c r="E189" s="16" t="s">
+        <v>465</v>
+      </c>
       <c r="F189" s="19">
         <v>180181182183184</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="6" t="s">
         <v>134</v>
       </c>
@@ -5590,12 +5706,14 @@
       <c r="D190" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E190" s="16"/>
+      <c r="E190" s="16" t="s">
+        <v>466</v>
+      </c>
       <c r="F190" s="19">
         <v>180181182183184</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A191" s="6" t="s">
         <v>134</v>
       </c>
@@ -5608,12 +5726,14 @@
       <c r="D191" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="E191" s="16"/>
+      <c r="E191" s="16" t="s">
+        <v>467</v>
+      </c>
       <c r="F191" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>134</v>
       </c>
@@ -5626,12 +5746,14 @@
       <c r="D192" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E192" s="16"/>
+      <c r="E192" s="16" t="s">
+        <v>469</v>
+      </c>
       <c r="F192" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
         <v>134</v>
       </c>
@@ -5644,7 +5766,9 @@
       <c r="D193" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E193" s="16"/>
+      <c r="E193" s="16" t="s">
+        <v>470</v>
+      </c>
       <c r="F193" s="14">
         <v>0</v>
       </c>
@@ -5662,12 +5786,14 @@
       <c r="D194" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="E194" s="16"/>
+      <c r="E194" s="16" t="s">
+        <v>471</v>
+      </c>
       <c r="F194" s="14">
         <v>186</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
         <v>134</v>
       </c>
@@ -5680,12 +5806,14 @@
       <c r="D195" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E195" s="16"/>
+      <c r="E195" s="16" t="s">
+        <v>473</v>
+      </c>
       <c r="F195" s="14">
         <v>191</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
         <v>134</v>
       </c>
@@ -5698,7 +5826,9 @@
       <c r="D196" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="E196" s="16"/>
+      <c r="E196" s="16" t="s">
+        <v>474</v>
+      </c>
       <c r="F196" s="14">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Environments Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="509">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1467,6 +1467,108 @@
   </si>
   <si>
     <t>Tests drive the release readiness while business drives the release decisions. A release candidate is only generated and available in the pipeline if all the tests have passed.</t>
+  </si>
+  <si>
+    <t>Data migrations are manually controlled. To move from this level data migration needs to be automated using frameworks such as SouthDB Migration.</t>
+  </si>
+  <si>
+    <t>Test data is not controllable. It is not generated and maintained by the team on demand but follows a very manual process to be generated.</t>
+  </si>
+  <si>
+    <t>Environments are heavily governed and regulated. Teams have no control over environments and several teams share environments.</t>
+  </si>
+  <si>
+    <t>Environments are stale and not refreshed regularly. Some of the critical tests environment are out of sync often. The environment refresh needs to be implemented and available on demand.</t>
+  </si>
+  <si>
+    <t>Test environments and test data are frequently unavailable to the teams that need them. The team depends on other teams to have both the data and environment available.</t>
+  </si>
+  <si>
+    <t>The different environments are provisioned manually by highly skilled individuals who are generally not part of the team. Requests for environments need to be raised and the process is not fast.</t>
+  </si>
+  <si>
+    <t>There are key person dependencies in the team. Absence of certain individuals leads to no access to certain environments required for the team to deploy the applications to such environments.</t>
+  </si>
+  <si>
+    <t>Data migrations are done with automated scripts that are versioned similar to the application code. These changes are tracked, monitored and reviewed regularly.</t>
+  </si>
+  <si>
+    <t>Separate test environments are available for the team. The team does not use the development environment as the test bed.</t>
+  </si>
+  <si>
+    <t>The test environment is shared by multiple teams. Changes to the environment requires a coordinated effort with the different teams.</t>
+  </si>
+  <si>
+    <t>Teams external to the development teams maintain the environments and are the only ones allowed to access and modify these environments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test environments are only available to the teams during particular dates or time slots. The team is forced to wait for the next slot if they miss a target slot and is unable to do ad hoc or continuous deployments into the test environment. </t>
+  </si>
+  <si>
+    <t>Teams can deploy basic virtual environments in controlled environments. They however do not have control over the actual environments.</t>
+  </si>
+  <si>
+    <t>There is a dedicated development environment for the teams.</t>
+  </si>
+  <si>
+    <t>Database migrations happen as part of deployment. The deployment pipelines have steps to ensure that the database base is in a state expected by the application. This scripts are idempotent in nature.</t>
+  </si>
+  <si>
+    <t>Test environments are readily available and can be reproduced to a predictable state. The steps are however not completely automated.</t>
+  </si>
+  <si>
+    <t>Provisioning is partially automated but there are still some manual configuration steps to get the environment to a functional state for the application.</t>
+  </si>
+  <si>
+    <t>Access to production-like environments are restricted. Requests are required to have these environments and can lead to bottlenecks</t>
+  </si>
+  <si>
+    <t>Some environments provide testable interfaces which can be used for the integration, functional, and non-functional type testing of the application.</t>
+  </si>
+  <si>
+    <t>Database migrations forward and backward are tested with every deployment.</t>
+  </si>
+  <si>
+    <t>The performance of the databases are monitored and optimized. The metrics are displayed on the team dashboards.</t>
+  </si>
+  <si>
+    <t>The environments can be replicated and reconfigured within a matter of hours after being destroyed. This, however, requires some manual work for configuration.</t>
+  </si>
+  <si>
+    <t>Multiple test environments are readily available for the exclusive use of the team, including a production-like environment that’s allows a reasonable level of non-functional and systems level testing. These environments are controlled by the teams.</t>
+  </si>
+  <si>
+    <t>Developer workstation set-up is automated. A new developer or technologist joining the team is able to set up their workstation by pulling the latest code base and running a few scripts.</t>
+  </si>
+  <si>
+    <t>Virtual environments are stubbed so integration and end-to-end type test can be run successfully.</t>
+  </si>
+  <si>
+    <t>Data and environment are versioned and managed in the version control management system in the same way as source code and artefacts.</t>
+  </si>
+  <si>
+    <t>Database performance is monitored and displayed on the team dashboards. This is tracked post-release and post-deployment and backlog items created if there are noticeable performance degradations.</t>
+  </si>
+  <si>
+    <t>Monitoring is proactive rather than reactive. The dashboards are displayed in a control room and performance thresholds are set for alerting purposes. Degradation of performance leads to task items which are prioritised and worked on.</t>
+  </si>
+  <si>
+    <t>Infrastructure Provisioning is part of the build pipeline as well as configuration enforcement. Tools such as Chef are used to enforce configuration of machine states and to automate the provisioning of infrastructure.</t>
+  </si>
+  <si>
+    <t>Teams manage their own infrastructure on demand and can provision and destroy infrastructure at will in line with their application requirements.</t>
+  </si>
+  <si>
+    <t>All environments are monitored and managed on a dashboard that shows the health and other status.</t>
+  </si>
+  <si>
+    <t>The provisioning of infrastructure is fully automated</t>
+  </si>
+  <si>
+    <t>Stubs are used to simulate dependencies where necessary.</t>
+  </si>
+  <si>
+    <t>Virtualization is used where applicable as opposed to physical hardware. Containerisation is also used where applicable.</t>
   </si>
 </sst>
 </file>
@@ -1899,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E197" sqref="E197"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E249" sqref="E249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5833,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
         <v>154</v>
       </c>
@@ -5846,12 +5948,14 @@
       <c r="D197" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="E197" s="16"/>
+      <c r="E197" s="16" t="s">
+        <v>475</v>
+      </c>
       <c r="F197" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>154</v>
       </c>
@@ -5864,12 +5968,14 @@
       <c r="D198" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E198" s="16"/>
+      <c r="E198" s="16" t="s">
+        <v>476</v>
+      </c>
       <c r="F198" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
         <v>154</v>
       </c>
@@ -5882,12 +5988,14 @@
       <c r="D199" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="E199" s="16"/>
+      <c r="E199" s="16" t="s">
+        <v>477</v>
+      </c>
       <c r="F199" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
         <v>154</v>
       </c>
@@ -5900,12 +6008,14 @@
       <c r="D200" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E200" s="16"/>
+      <c r="E200" s="16" t="s">
+        <v>478</v>
+      </c>
       <c r="F200" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A201" s="6" t="s">
         <v>154</v>
       </c>
@@ -5918,12 +6028,14 @@
       <c r="D201" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E201" s="16"/>
+      <c r="E201" s="16" t="s">
+        <v>479</v>
+      </c>
       <c r="F201" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
         <v>154</v>
       </c>
@@ -5936,12 +6048,14 @@
       <c r="D202" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="E202" s="16"/>
+      <c r="E202" s="16" t="s">
+        <v>480</v>
+      </c>
       <c r="F202" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
         <v>154</v>
       </c>
@@ -5954,12 +6068,14 @@
       <c r="D203" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E203" s="17"/>
+      <c r="E203" s="17" t="s">
+        <v>481</v>
+      </c>
       <c r="F203" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
         <v>154</v>
       </c>
@@ -5972,12 +6088,14 @@
       <c r="D204" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="E204" s="17"/>
+      <c r="E204" s="17" t="s">
+        <v>482</v>
+      </c>
       <c r="F204" s="14">
         <v>197</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
         <v>154</v>
       </c>
@@ -5990,12 +6108,14 @@
       <c r="D205" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="E205" s="17"/>
+      <c r="E205" s="17" t="s">
+        <v>483</v>
+      </c>
       <c r="F205" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
         <v>154</v>
       </c>
@@ -6008,12 +6128,14 @@
       <c r="D206" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="E206" s="17"/>
+      <c r="E206" s="17" t="s">
+        <v>484</v>
+      </c>
       <c r="F206" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A207" s="6" t="s">
         <v>154</v>
       </c>
@@ -6026,12 +6148,14 @@
       <c r="D207" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E207" s="17"/>
+      <c r="E207" s="17" t="s">
+        <v>485</v>
+      </c>
       <c r="F207" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A208" s="6" t="s">
         <v>154</v>
       </c>
@@ -6044,12 +6168,14 @@
       <c r="D208" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E208" s="17"/>
+      <c r="E208" s="17" t="s">
+        <v>486</v>
+      </c>
       <c r="F208" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
         <v>154</v>
       </c>
@@ -6062,7 +6188,9 @@
       <c r="D209" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E209" s="17"/>
+      <c r="E209" s="17" t="s">
+        <v>487</v>
+      </c>
       <c r="F209" s="14">
         <v>0</v>
       </c>
@@ -6080,12 +6208,14 @@
       <c r="D210" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="E210" s="17"/>
+      <c r="E210" s="17" t="s">
+        <v>488</v>
+      </c>
       <c r="F210" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A211" s="6" t="s">
         <v>154</v>
       </c>
@@ -6098,7 +6228,9 @@
       <c r="D211" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E211" s="17"/>
+      <c r="E211" s="17" t="s">
+        <v>489</v>
+      </c>
       <c r="F211" s="14">
         <v>204</v>
       </c>
@@ -6116,7 +6248,9 @@
       <c r="D212" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E212" s="17"/>
+      <c r="E212" s="17" t="s">
+        <v>490</v>
+      </c>
       <c r="F212" s="19">
         <v>205206207208</v>
       </c>
@@ -6134,12 +6268,14 @@
       <c r="D213" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E213" s="17"/>
+      <c r="E213" s="17" t="s">
+        <v>492</v>
+      </c>
       <c r="F213" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A214" s="6" t="s">
         <v>154</v>
       </c>
@@ -6152,7 +6288,9 @@
       <c r="D214" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E214" s="17"/>
+      <c r="E214" s="17" t="s">
+        <v>491</v>
+      </c>
       <c r="F214" s="14">
         <v>202</v>
       </c>
@@ -6170,12 +6308,14 @@
       <c r="D215" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E215" s="17"/>
+      <c r="E215" s="17" t="s">
+        <v>493</v>
+      </c>
       <c r="F215" s="14">
         <v>209</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" s="6" t="s">
         <v>154</v>
       </c>
@@ -6188,12 +6328,14 @@
       <c r="D216" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="E216" s="17"/>
+      <c r="E216" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="F216" s="14">
         <v>211</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A217" s="6" t="s">
         <v>154</v>
       </c>
@@ -6206,12 +6348,14 @@
       <c r="D217" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="E217" s="17"/>
+      <c r="E217" s="17" t="s">
+        <v>495</v>
+      </c>
       <c r="F217" s="14">
         <v>211</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A218" s="6" t="s">
         <v>154</v>
       </c>
@@ -6224,7 +6368,9 @@
       <c r="D218" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="E218" s="17"/>
+      <c r="E218" s="17" t="s">
+        <v>496</v>
+      </c>
       <c r="F218" s="19">
         <v>212213</v>
       </c>
@@ -6242,12 +6388,14 @@
       <c r="D219" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="E219" s="17"/>
+      <c r="E219" s="17" t="s">
+        <v>497</v>
+      </c>
       <c r="F219" s="19">
         <v>212213</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A220" s="6" t="s">
         <v>154</v>
       </c>
@@ -6260,7 +6408,9 @@
       <c r="D220" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="E220" s="17"/>
+      <c r="E220" s="17" t="s">
+        <v>498</v>
+      </c>
       <c r="F220" s="14">
         <v>0</v>
       </c>
@@ -6278,7 +6428,9 @@
       <c r="D221" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E221" s="17"/>
+      <c r="E221" s="17" t="s">
+        <v>499</v>
+      </c>
       <c r="F221" s="14">
         <v>215</v>
       </c>
@@ -6296,7 +6448,9 @@
       <c r="D222" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="E222" s="17"/>
+      <c r="E222" s="17" t="s">
+        <v>500</v>
+      </c>
       <c r="F222" s="19">
         <v>216217</v>
       </c>
@@ -6314,12 +6468,14 @@
       <c r="D223" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="E223" s="17"/>
+      <c r="E223" s="17" t="s">
+        <v>501</v>
+      </c>
       <c r="F223" s="19">
         <v>216217</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
         <v>154</v>
       </c>
@@ -6332,12 +6488,14 @@
       <c r="D224" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="E224" s="17"/>
+      <c r="E224" s="17" t="s">
+        <v>502</v>
+      </c>
       <c r="F224" s="19">
         <v>216217</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A225" s="6" t="s">
         <v>154</v>
       </c>
@@ -6350,7 +6508,9 @@
       <c r="D225" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="E225" s="17"/>
+      <c r="E225" s="17" t="s">
+        <v>503</v>
+      </c>
       <c r="F225" s="19">
         <v>218219</v>
       </c>
@@ -6368,12 +6528,14 @@
       <c r="D226" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="E226" s="17"/>
+      <c r="E226" s="17" t="s">
+        <v>504</v>
+      </c>
       <c r="F226" s="19">
         <v>218219</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
         <v>154</v>
       </c>
@@ -6386,7 +6548,9 @@
       <c r="D227" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="E227" s="17"/>
+      <c r="E227" s="17" t="s">
+        <v>505</v>
+      </c>
       <c r="F227" s="19">
         <v>218219</v>
       </c>
@@ -6404,7 +6568,9 @@
       <c r="D228" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="E228" s="17"/>
+      <c r="E228" s="17" t="s">
+        <v>506</v>
+      </c>
       <c r="F228" s="14">
         <v>214</v>
       </c>
@@ -6422,12 +6588,14 @@
       <c r="D229" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="E229" s="17"/>
+      <c r="E229" s="17" t="s">
+        <v>507</v>
+      </c>
       <c r="F229" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A230" s="6" t="s">
         <v>154</v>
       </c>
@@ -6440,7 +6608,9 @@
       <c r="D230" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="E230" s="17"/>
+      <c r="E230" s="17" t="s">
+        <v>508</v>
+      </c>
       <c r="F230" s="14">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
Brain: Completing the Acceptance Criteria for Feature Teaming Capability
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="527">
   <si>
     <t xml:space="preserve">Dimension Name </t>
   </si>
@@ -1569,6 +1569,60 @@
   </si>
   <si>
     <t>Virtualization is used where applicable as opposed to physical hardware. Containerisation is also used where applicable.</t>
+  </si>
+  <si>
+    <t>At this level the team is not cross-functional in nature. Some of the skills required to complete end-to-end customer features are missing and there is dependence of teams/people outside the team.</t>
+  </si>
+  <si>
+    <t>Team members are not 100% allocated to the teams and have other priorities as well that they have to allocate their time to.</t>
+  </si>
+  <si>
+    <t>Collaboration between team members is low at this mastery level and mainly ad hoc.</t>
+  </si>
+  <si>
+    <t>Software release requires multiple handoffs and dependency on external teams and stakeholders. The team does not know the different external teams and stake holders and the handoffs are not transparent to the team.</t>
+  </si>
+  <si>
+    <t>The team has access to cross-functional skills and cross-component skills even though these skills are not embedded in the teams. These skills are readily available to assist the team in delivering the functionality. For example the team can access quality assurance engineers as needed without them being embedded in the team.</t>
+  </si>
+  <si>
+    <t>All the handoffs are identified and mapped on the team deployment/release process document.</t>
+  </si>
+  <si>
+    <t>The concept of triads is established in the team and is respected for features to be considered as done. Business, Technical and Quality are committed to execute the strategy together.</t>
+  </si>
+  <si>
+    <t>Team member allocations are 100% to the team.</t>
+  </si>
+  <si>
+    <t>Cross-functional and cross-component skills are embedded in the teams and all the requisite skills required to deliver end-to-end customer value are embedded in the teams. There is no external team dependency to deliver the goals and vision of the product.</t>
+  </si>
+  <si>
+    <t>An onboarding plan for new members exists and this is maintained and reviewed often. The onboarding plan is documented and accessible on the document management application.</t>
+  </si>
+  <si>
+    <t>The triad (business, technology and quality) is fully functional in the teams and the product owners within the teams are empowered to make the decisions pertaining to the product roadmap with need of external consultation or validation.</t>
+  </si>
+  <si>
+    <t>The product goals are clearly prioritized and recorded on the team document management system and the top priority goals are visual on the team walls.</t>
+  </si>
+  <si>
+    <t>Team members can perform more than one function. For example, the developers can serve as quality engineers.</t>
+  </si>
+  <si>
+    <t>Team has autonomy and is self-organized. The team composition is well understood by all team members and stakeholders and the roles are responsibilities are clearly defined and understood.</t>
+  </si>
+  <si>
+    <t>Kaizen (constant improvement) is performed by the team every iteration. The team collects metrics, which are radiated on the wall and regularly holds retrospectives with action items visible on the team wall towards continuous improvement.</t>
+  </si>
+  <si>
+    <t>A majority of the team is comprised of individuals who can play dual roles and there is collective shared responsibility by the team members. Failure or success is team failure or success.</t>
+  </si>
+  <si>
+    <t>The team is in charge of the end-to-end delivery of the product from infrastructure, to configuration, to application deployment to instrumentation and alerting.</t>
+  </si>
+  <si>
+    <t>Team performs restrospectives every iteration to drive continuous improvements.</t>
   </si>
 </sst>
 </file>
@@ -2001,8 +2055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E249" sqref="E249"/>
+    <sheetView tabSelected="1" topLeftCell="A242" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E250" sqref="E250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6615,7 +6669,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A231" s="6" t="s">
         <v>183</v>
       </c>
@@ -6628,12 +6682,14 @@
       <c r="D231" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="E231" s="17"/>
+      <c r="E231" s="17" t="s">
+        <v>509</v>
+      </c>
       <c r="F231" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A232" s="6" t="s">
         <v>183</v>
       </c>
@@ -6646,12 +6702,14 @@
       <c r="D232" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="E232" s="17"/>
+      <c r="E232" s="17" t="s">
+        <v>510</v>
+      </c>
       <c r="F232" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A233" s="6" t="s">
         <v>183</v>
       </c>
@@ -6664,12 +6722,14 @@
       <c r="D233" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="E233" s="17"/>
+      <c r="E233" s="17" t="s">
+        <v>511</v>
+      </c>
       <c r="F233" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A234" s="6" t="s">
         <v>183</v>
       </c>
@@ -6682,12 +6742,14 @@
       <c r="D234" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="E234" s="17"/>
+      <c r="E234" s="17" t="s">
+        <v>512</v>
+      </c>
       <c r="F234" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
         <v>183</v>
       </c>
@@ -6700,12 +6762,14 @@
       <c r="D235" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="E235" s="17"/>
+      <c r="E235" s="17" t="s">
+        <v>513</v>
+      </c>
       <c r="F235" s="19">
         <v>231232</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A236" s="6" t="s">
         <v>183</v>
       </c>
@@ -6718,7 +6782,9 @@
       <c r="D236" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="E236" s="17"/>
+      <c r="E236" s="17" t="s">
+        <v>514</v>
+      </c>
       <c r="F236" s="14">
         <v>234</v>
       </c>
@@ -6736,7 +6802,9 @@
       <c r="D237" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="E237" s="17"/>
+      <c r="E237" s="17" t="s">
+        <v>515</v>
+      </c>
       <c r="F237" s="14">
         <v>0</v>
       </c>
@@ -6754,12 +6822,14 @@
       <c r="D238" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="E238" s="17"/>
+      <c r="E238" s="17" t="s">
+        <v>516</v>
+      </c>
       <c r="F238" s="14">
         <v>232</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A239" s="6" t="s">
         <v>183</v>
       </c>
@@ -6772,12 +6842,14 @@
       <c r="D239" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="E239" s="17"/>
+      <c r="E239" s="17" t="s">
+        <v>517</v>
+      </c>
       <c r="F239" s="14">
         <v>235</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A240" s="6" t="s">
         <v>183</v>
       </c>
@@ -6790,12 +6862,14 @@
       <c r="D240" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="E240" s="17"/>
+      <c r="E240" s="17" t="s">
+        <v>518</v>
+      </c>
       <c r="F240" s="14">
         <v>235</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A241" s="6" t="s">
         <v>183</v>
       </c>
@@ -6808,12 +6882,14 @@
       <c r="D241" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="E241" s="17"/>
+      <c r="E241" s="17" t="s">
+        <v>519</v>
+      </c>
       <c r="F241" s="14">
         <v>237</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A242" s="6" t="s">
         <v>183</v>
       </c>
@@ -6826,7 +6902,9 @@
       <c r="D242" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E242" s="3"/>
+      <c r="E242" s="3" t="s">
+        <v>520</v>
+      </c>
       <c r="F242" s="14">
         <v>0</v>
       </c>
@@ -6844,7 +6922,9 @@
       <c r="D243" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="E243" s="16"/>
+      <c r="E243" s="16" t="s">
+        <v>521</v>
+      </c>
       <c r="F243" s="19">
         <v>239240</v>
       </c>
@@ -6862,12 +6942,14 @@
       <c r="D244" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="E244" s="16"/>
+      <c r="E244" s="16" t="s">
+        <v>522</v>
+      </c>
       <c r="F244" s="19">
         <v>239240</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A245" s="6" t="s">
         <v>183</v>
       </c>
@@ -6880,12 +6962,14 @@
       <c r="D245" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E245" s="3"/>
+      <c r="E245" s="3" t="s">
+        <v>523</v>
+      </c>
       <c r="F245" s="14">
         <v>242</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
         <v>183</v>
       </c>
@@ -6898,12 +6982,14 @@
       <c r="D246" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="E246" s="16"/>
+      <c r="E246" s="16" t="s">
+        <v>426</v>
+      </c>
       <c r="F246" s="19">
         <v>243244</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A247" s="6" t="s">
         <v>183</v>
       </c>
@@ -6916,12 +7002,14 @@
       <c r="D247" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="E247" s="16"/>
+      <c r="E247" s="16" t="s">
+        <v>524</v>
+      </c>
       <c r="F247" s="19">
         <v>243244</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A248" s="6" t="s">
         <v>183</v>
       </c>
@@ -6934,7 +7022,9 @@
       <c r="D248" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E248" s="16"/>
+      <c r="E248" s="16" t="s">
+        <v>525</v>
+      </c>
       <c r="F248" s="19">
         <v>243244</v>
       </c>
@@ -6952,7 +7042,9 @@
       <c r="D249" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E249" s="3"/>
+      <c r="E249" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="F249" s="14">
         <v>245</v>
       </c>

</xml_diff>

<commit_message>
Brain: Edit of grammatical errors
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -872,18 +872,12 @@
     <t>Acceptance Criteria</t>
   </si>
   <si>
-    <t>There is no explicit definition of the strategy in the teams. The team do not have a shared accessible document where they can see the strategy. Alignement is purely coincidental and not deliberate</t>
-  </si>
-  <si>
     <t>Business and Technology stakeholders are both present in the PI Planning sessions. The team engages with both the business and technical stakeholders for the strategy and goal setting.</t>
   </si>
   <si>
     <t>The team has access to the product/project vision as well as the strategy. There is clear visualisation of how the vision aligns to the strategy and all the team members can access the document that links the two.</t>
   </si>
   <si>
-    <t>There is a review of alignement to strategy in the Post implementation PI sessions but no review during the implementation stage.</t>
-  </si>
-  <si>
     <t>The team engages with the stake holders during implementation to ensure business and technical alignment. This engagement is however occasional for example once every 2 months or so.</t>
   </si>
   <si>
@@ -962,9 +956,6 @@
     <t>Acceptance criteria are used for the stories to be worked on. The requirements are not done many months before the work is performed but rather one or two iterations in advance.</t>
   </si>
   <si>
-    <t>There is visible innovation/optimisation in the team in line with the strategy. These are captured as cards on the teams story wall and extra achievements in the scope management tool.</t>
-  </si>
-  <si>
     <t>A lists is maintained of stories that have been completed as well as stories that have gone through the flow and had to be sent back to analysis after showcase.</t>
   </si>
   <si>
@@ -974,9 +965,6 @@
     <t>Team caters for technical debt as part of the normal workflow lifecycle. Stories are created for such technical debt in the backlog and these are prioritised, planned and executed in the same flow as other business relevant stories. Stakeholders are informed of the significance and impact of the technical debt.</t>
   </si>
   <si>
-    <t>The retrospectives are run every iteration and the stakeholders are present in the retrospective. Stakeholders contribute to retrospectives and action items which are allocated to them are tracked by the team on the team wall.</t>
-  </si>
-  <si>
     <t>The requirements on the backlog have acceptance criteria with clear outcomes and objective measures of what success is.</t>
   </si>
   <si>
@@ -1025,15 +1013,6 @@
     <t>The team reviews the processes and practices every iteration. Quality threshold metrics are increased and the processes are optimized.</t>
   </si>
   <si>
-    <t>There are continuous assessments of the code metrics to ensure the team is aligned to the quality standards. Backlog items are created to address gaps identified from the code metrics perspective and these are tracked and prioritized.</t>
-  </si>
-  <si>
-    <t>Technical debt items are tracked and the code static analysis metrics are tracked to show progress with technical debt reduction.</t>
-  </si>
-  <si>
-    <t>Artefacts, code and report are kept in developer machines. There is no use of a version management technology.</t>
-  </si>
-  <si>
     <t>All deployments and application rollbacks are done manually by experienced developers or operations.</t>
   </si>
   <si>
@@ -1046,12 +1025,6 @@
     <t>All the testing performed are manual, predominantly exploratory type tests. Team needs to start implementing automated tests.</t>
   </si>
   <si>
-    <t>The environments required by the development teams (developers, QAs, UAT etc) are provisioned manually and shared by multiple teams. The team is unable to modify configuration which they want to test adhoc and needs to raise change requests.</t>
-  </si>
-  <si>
-    <t>The source code is checked in to a version control tool even though the team commits are very infrequent.</t>
-  </si>
-  <si>
     <t>There's a script to build the application and this process is automated. There are also tests run as part of the build process.</t>
   </si>
   <si>
@@ -1065,9 +1038,6 @@
   </si>
   <si>
     <t>Builds are triggered by simple click of a button on the continuous integration management tool.</t>
-  </si>
-  <si>
-    <t>Build status are shown on dashboards which the team can see. Team has a view of the broken builds history. Team continues with coding tasks even when the build is broken. The team needs to start moving towards a state where a broken build leads to a stop in new functionality until the build is fixed (Think Broken Window Syndrome).</t>
   </si>
   <si>
     <t>The test coverage is greater than 50% but not entirely covered. Team needs to improve on the test coverage and move it towards 90 - 100% coverage. Team fails the build if the coverage metric is not met.</t>
@@ -1151,9 +1121,6 @@
     <t>There are key people identified to handle incidents and this is well known by the team.</t>
   </si>
   <si>
-    <t>There is very minimal handoffs. The resolution is effective and insolves very few teams, generally the core team and the dependent system team.</t>
-  </si>
-  <si>
     <t>The incidents are recorded in the team backlog and prioritised together with all the other work in flight. There is an understanding of incident classification and the turn around time for the different classes of incidents. The team reacts appropriately based on the class of the incident.</t>
   </si>
   <si>
@@ -1202,9 +1169,6 @@
     <t>At this level, risks are captured by the team and tracked on the team wall and/or story management system. The team members can access the various risks and are all aware of what they are.</t>
   </si>
   <si>
-    <t>The risks are allocated owners as well as mititgation/action plans. These are clearly captured in the story management system.</t>
-  </si>
-  <si>
     <t>The risks are discussed and reviewed as part of the iteration planning process and action items are allocated and assigned to prospective risk item owners. These are then tracked and reviewed throughout the iteration to ensure mitigation is in place.</t>
   </si>
   <si>
@@ -1220,9 +1184,6 @@
     <t>Cost benefit analysis of risk mitigations are discussed in the iteration planning sessions before risks are prioritised.</t>
   </si>
   <si>
-    <t>Roles, responsibilities and accountabilities for the risks owners are defined, agreed upon and documented where it is accessible by all team members.</t>
-  </si>
-  <si>
     <t>There is clear communication with the business stakeholders and different stakeholders on the risks and mitigation plans in progress.</t>
   </si>
   <si>
@@ -1244,9 +1205,6 @@
     <t>Design and technical decisions are done in an adhoc manner with no vision of the application road map. Technical team members are not aware of the overall technical design decisions and this is not documented in any form.</t>
   </si>
   <si>
-    <t>At this level of proficiency, the team does a lot of Big Up-Front designs for the systems as opposed to a just enough design approach. There are several ceremonial design sessions for the entire application without necessarily taken into effect the fact that there might need to be changes should the product vision change.</t>
-  </si>
-  <si>
     <t>Technologists at this level of proficiency design highly tightly coupled and brittle systems. The goal should be to start designing loosely coupled systems so that they are independently deployable and can be monitored in isolation.</t>
   </si>
   <si>
@@ -1256,18 +1214,12 @@
     <t>Design assumptions are tracked and recorded on the team wall and these are validated during the iteration as well as during the iteration planning sessions.</t>
   </si>
   <si>
-    <t>Design issues identified are tracked and prioritised in the backlog and attended to similar to the technical debts.</t>
-  </si>
-  <si>
     <t>The system non-functional requirements are documented and tracked. These are also prioritised in the backlog.</t>
   </si>
   <si>
     <t>The team emphasizes a modular design of the application with clearly defined interfaces between the modules and clear communication protocols between the modules (for example clearly defined APIs using RESTful protocols).</t>
   </si>
   <si>
-    <t>The technical design is owned by the feature teams. The technical architect is part of the core team and is not a stakeholder external to the team making decisions on their behalf.</t>
-  </si>
-  <si>
     <t>Some design decisions can be linked to the requirements, however, not all the design decisions are.</t>
   </si>
   <si>
@@ -1292,9 +1244,6 @@
     <t>The teams at this level of proficiency do not have autonomy with respect to decision making. They need to consult for any decisions they make and cannot be qualified as autonomous teams. To move from this level teams need to start making their own decisions and have some autonomy.</t>
   </si>
   <si>
-    <t>The teams work of functionality without necessarily knowing what the goal and vision is. Some people in the team or some stakeholders may know the vision but this is not shared across and this has not been documented. The goals/vision need to be documented and easily accessible.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Few individuals in the team understand the stakeholder landscape but the whole team is unaware of the entire stakeholder landscape. </t>
   </si>
   <si>
@@ -1346,12 +1295,6 @@
     <t>The team is able to plan releases to a regular cycle and can track and manage features within regular time frames. Delivery is more predictable and captured on the team walls.</t>
   </si>
   <si>
-    <t>The release dates are seldom moved out. The team is able to rather reduce the release features rather than the move out the release dates.</t>
-  </si>
-  <si>
-    <t>There is a well defined process for handling the release of the artefacts to operations and support teams in places. This is documented and well understood by all the team members. The team at this level is investigating means of embedding operations/support in the team structure.</t>
-  </si>
-  <si>
     <t>Build artefacts are well defined and produced preferably by the build/continuous integration tool. These artefacts are readily available to the team as well as the operations and support teams. The team is able to tell which artefact was deployed when.</t>
   </si>
   <si>
@@ -1511,9 +1454,6 @@
     <t>There is a dedicated development environment for the teams.</t>
   </si>
   <si>
-    <t>Database migrations happen as part of deployment. The deployment pipelines have steps to ensure that the database base is in a state expected by the application. This scripts are idempotent in nature.</t>
-  </si>
-  <si>
     <t>Test environments are readily available and can be reproduced to a predictable state. The steps are however not completely automated.</t>
   </si>
   <si>
@@ -1535,18 +1475,12 @@
     <t>The environments can be replicated and reconfigured within a matter of hours after being destroyed. This, however, requires some manual work for configuration.</t>
   </si>
   <si>
-    <t>Multiple test environments are readily available for the exclusive use of the team, including a production-like environment that’s allows a reasonable level of non-functional and systems level testing. These environments are controlled by the teams.</t>
-  </si>
-  <si>
     <t>Developer workstation set-up is automated. A new developer or technologist joining the team is able to set up their workstation by pulling the latest code base and running a few scripts.</t>
   </si>
   <si>
     <t>Virtual environments are stubbed so integration and end-to-end type test can be run successfully.</t>
   </si>
   <si>
-    <t>Data and environment are versioned and managed in the version control management system in the same way as source code and artefacts.</t>
-  </si>
-  <si>
     <t>Database performance is monitored and displayed on the team dashboards. This is tracked post-release and post-deployment and backlog items created if there are noticeable performance degradations.</t>
   </si>
   <si>
@@ -1571,9 +1505,6 @@
     <t>Virtualization is used where applicable as opposed to physical hardware. Containerisation is also used where applicable.</t>
   </si>
   <si>
-    <t>At this level the team is not cross-functional in nature. Some of the skills required to complete end-to-end customer features are missing and there is dependence of teams/people outside the team.</t>
-  </si>
-  <si>
     <t>Team members are not 100% allocated to the teams and have other priorities as well that they have to allocate their time to.</t>
   </si>
   <si>
@@ -1595,24 +1526,15 @@
     <t>Team member allocations are 100% to the team.</t>
   </si>
   <si>
-    <t>Cross-functional and cross-component skills are embedded in the teams and all the requisite skills required to deliver end-to-end customer value are embedded in the teams. There is no external team dependency to deliver the goals and vision of the product.</t>
-  </si>
-  <si>
     <t>An onboarding plan for new members exists and this is maintained and reviewed often. The onboarding plan is documented and accessible on the document management application.</t>
   </si>
   <si>
-    <t>The triad (business, technology and quality) is fully functional in the teams and the product owners within the teams are empowered to make the decisions pertaining to the product roadmap with need of external consultation or validation.</t>
-  </si>
-  <si>
     <t>The product goals are clearly prioritized and recorded on the team document management system and the top priority goals are visual on the team walls.</t>
   </si>
   <si>
     <t>Team members can perform more than one function. For example, the developers can serve as quality engineers.</t>
   </si>
   <si>
-    <t>Team has autonomy and is self-organized. The team composition is well understood by all team members and stakeholders and the roles are responsibilities are clearly defined and understood.</t>
-  </si>
-  <si>
     <t>Kaizen (constant improvement) is performed by the team every iteration. The team collects metrics, which are radiated on the wall and regularly holds retrospectives with action items visible on the team wall towards continuous improvement.</t>
   </si>
   <si>
@@ -1623,6 +1545,84 @@
   </si>
   <si>
     <t>Team performs restrospectives every iteration to drive continuous improvements.</t>
+  </si>
+  <si>
+    <t>There is no explicit definition of the strategy in the teams. The team does not have a shared accessible document where they can see the strategy. Alignement is purely coincidental and not deliberate</t>
+  </si>
+  <si>
+    <t>There is a review of alignment to strategy in the Post implementation PI sessions but no review during the implementation stage.</t>
+  </si>
+  <si>
+    <t>There is visible innovation/optimisation in the team in line with the strategy. These are captured as cards on the team's story wall and as extra achievements in the scope management tool.</t>
+  </si>
+  <si>
+    <t>The retrospectives are run every iteration and the stakeholders are present in the retrospectives. Stakeholders contribute to retrospectives and action items, which are allocated to them are tracked by the team on the team wall.</t>
+  </si>
+  <si>
+    <t>There are continuous assessments of the code metrics to ensure the team is aligned to the quality standards. Backlog items are created to address gaps identified from the code metrics' perspective and these are tracked and prioritized.</t>
+  </si>
+  <si>
+    <t>Technical debt items are tracked and the code static analysis metrics are tracked to show progress with respect to technical debt reduction.</t>
+  </si>
+  <si>
+    <t>Artefacts, code and reports are kept in developer machines. There is no use of a version management technology.</t>
+  </si>
+  <si>
+    <t>The environments required by the development teams (developers, QAs, UAT etc) are provisioned manually and shared by multiple teams. The team is unable to modify configuration which they want to test ad hoc and needs to raise change requests.</t>
+  </si>
+  <si>
+    <t>The source code is checked in to a version control management tool even though the team commits are very infrequent.</t>
+  </si>
+  <si>
+    <t>Build statuses are shown on dashboards which the team can see. Team has a view of the broken builds history. Team continues with coding tasks even when the build is broken. The team needs to start moving towards a state where a broken build leads to a stop in new functionality until the build is fixed (Think Broken Window Syndrome).</t>
+  </si>
+  <si>
+    <t>There is very minimal handoffs. The resolution is effective and involves very few teams, generally the core team and the dependent system team.</t>
+  </si>
+  <si>
+    <t>The risks are allocated owners as well as mitigation/action plans. These are clearly captured in the story management system.</t>
+  </si>
+  <si>
+    <t>Roles, responsibilities and accountabilities for the risks owners are defined, agreed upon and documented where it is accessible to all team members.</t>
+  </si>
+  <si>
+    <t>At this level of proficiency, the team does a lot of Big Up-Front designs for the systems as opposed to a "just enough" design approach. There are several ceremonial design sessions for the entire application without necessarily taking into effect the fact that there might need to be changes should the product vision change.</t>
+  </si>
+  <si>
+    <t>Design issues identified are tracked and prioritised in the backlog and attended to, similar to the technical debts.</t>
+  </si>
+  <si>
+    <t>The technical design is owned by the feature teams. The technical architect is part of the core team and is not a stakeholder, external to the team and making decisions on their behalf.</t>
+  </si>
+  <si>
+    <t>The teams work on functionality without necessarily knowing what the goal and vision is. Some people in the team or some stakeholders may know the vision but this is not shared across and this has not been documented. The goals/vision need to be documented and easily accessible.</t>
+  </si>
+  <si>
+    <t>The release dates are seldom moved out. The team is able to reduce the release features rather than the move out the release dates.</t>
+  </si>
+  <si>
+    <t>There is a well defined process for handling the release of the artefacts to operations and support teams in place. This is documented and well understood by all the team members. The team at this level is investigating means of embedding operations/support in the team structure.</t>
+  </si>
+  <si>
+    <t>Database migrations happen as part of deployment. The deployment pipelines have steps to ensure that the database base is in a state expected by the application. These scripts are idempotent in nature.</t>
+  </si>
+  <si>
+    <t>Multiple test environments are readily available for the exclusive use of the team, including a production-like environment that allows a reasonable level of non-functional and systems level testing. These environments are controlled by the teams.</t>
+  </si>
+  <si>
+    <t>Data and environments are versioned and managed in the version control management system in the same way as source code and artefacts.</t>
+  </si>
+  <si>
+    <t>At this level the team is not cross-functional in nature. Some of the skills required to complete end-to-end customer features are missing and there is dependence on teams/people outside the team.</t>
+  </si>
+  <si>
+    <t>Cross-functional and cross-component skills are embedded in the teams and all the requisite skills required to deliver end-to-end customer value are embedded in the teams. There is no external team dependency required to deliver the goals and vision of the product.</t>
+  </si>
+  <si>
+    <t>The triad (business, technology and quality) is fully functional in the teams and the product owners within the teams are empowered to make the decisions pertaining to the product roadmap without the need of external consultation or validation.</t>
+  </si>
+  <si>
+    <t>Team has autonomy and is self-organized. The team composition is well understood by all team members and stakeholders, and the roles and responsibilities are clearly defined and understood.</t>
   </si>
 </sst>
 </file>
@@ -2055,7 +2055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="E250" sqref="E250"/>
     </sheetView>
   </sheetViews>
@@ -2103,7 +2103,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>280</v>
+        <v>501</v>
       </c>
       <c r="F2" s="9">
         <v>0</v>
@@ -2123,7 +2123,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F3" s="9">
         <v>1</v>
@@ -2143,7 +2143,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F4" s="9">
         <v>1</v>
@@ -2163,7 +2163,7 @@
         <v>232</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>283</v>
+        <v>502</v>
       </c>
       <c r="F5" s="9">
         <v>1</v>
@@ -2183,7 +2183,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>18</v>
@@ -2203,7 +2203,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F7" s="9">
         <v>0</v>
@@ -2223,7 +2223,7 @@
         <v>204</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F8" s="9">
         <v>5</v>
@@ -2243,7 +2243,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F9" s="9">
         <v>5</v>
@@ -2263,7 +2263,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F10" s="9">
         <v>0</v>
@@ -2283,7 +2283,7 @@
         <v>205</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F11" s="9">
         <v>6</v>
@@ -2303,7 +2303,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F12" s="9">
         <v>9</v>
@@ -2323,7 +2323,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F13" s="9">
         <v>9</v>
@@ -2343,7 +2343,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>310</v>
+        <v>503</v>
       </c>
       <c r="F14" s="9">
         <v>9</v>
@@ -2363,7 +2363,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F15" s="9">
         <v>0</v>
@@ -2383,7 +2383,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F16" s="14">
         <v>0</v>
@@ -2403,7 +2403,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F17" s="9">
         <v>0</v>
@@ -2423,7 +2423,7 @@
         <v>213</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F18" s="9">
         <v>0</v>
@@ -2443,7 +2443,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F19" s="14">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>214</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F20" s="9">
         <v>14</v>
@@ -2483,7 +2483,7 @@
         <v>23</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F21" s="9">
         <v>15</v>
@@ -2503,7 +2503,7 @@
         <v>24</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F22" s="9">
         <v>16</v>
@@ -2523,7 +2523,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F23" s="9">
         <v>17</v>
@@ -2543,7 +2543,7 @@
         <v>230</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F24" s="9">
         <v>18</v>
@@ -2563,7 +2563,7 @@
         <v>26</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F25" s="9">
         <v>19</v>
@@ -2583,7 +2583,7 @@
         <v>243</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F26" s="9">
         <v>19</v>
@@ -2603,7 +2603,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F27" s="9">
         <v>20</v>
@@ -2623,7 +2623,7 @@
         <v>28</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F28" s="9">
         <v>22</v>
@@ -2643,7 +2643,7 @@
         <v>29</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F29" s="9">
         <v>0</v>
@@ -2663,7 +2663,7 @@
         <v>30</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F30" s="9">
         <v>23</v>
@@ -2683,7 +2683,7 @@
         <v>206</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>245</v>
@@ -2703,7 +2703,7 @@
         <v>207</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F32" s="9">
         <v>26</v>
@@ -2723,7 +2723,7 @@
         <v>208</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F33" s="9">
         <v>26</v>
@@ -2743,7 +2743,7 @@
         <v>209</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F34" s="9">
         <v>27</v>
@@ -2763,7 +2763,7 @@
         <v>229</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F35" s="9">
         <v>28</v>
@@ -2783,7 +2783,7 @@
         <v>210</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>314</v>
+        <v>504</v>
       </c>
       <c r="F36" s="9">
         <v>29</v>
@@ -2803,7 +2803,7 @@
         <v>31</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>244</v>
@@ -2823,7 +2823,7 @@
         <v>32</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>246</v>
@@ -2843,7 +2843,7 @@
         <v>231</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F39" s="9">
         <v>35</v>
@@ -2863,7 +2863,7 @@
         <v>35</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F40" s="9">
         <v>0</v>
@@ -2883,7 +2883,7 @@
         <v>247</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F41" s="9">
         <v>39</v>
@@ -2903,7 +2903,7 @@
         <v>224</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F42" s="9">
         <v>0</v>
@@ -2923,7 +2923,7 @@
         <v>36</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F43" s="9">
         <v>40</v>
@@ -2943,7 +2943,7 @@
         <v>37</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F44" s="9">
         <v>41</v>
@@ -2963,7 +2963,7 @@
         <v>38</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F45" s="9">
         <v>0</v>
@@ -2983,7 +2983,7 @@
         <v>39</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F46" s="9">
         <v>0</v>
@@ -3003,7 +3003,7 @@
         <v>40</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F47" s="9">
         <v>44</v>
@@ -3023,7 +3023,7 @@
         <v>41</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F48" s="9">
         <v>44</v>
@@ -3043,7 +3043,7 @@
         <v>42</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F49" s="9">
         <v>45</v>
@@ -3063,7 +3063,7 @@
         <v>43</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F50" s="9">
         <v>45</v>
@@ -3083,7 +3083,7 @@
         <v>44</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F51" s="9">
         <v>42</v>
@@ -3103,7 +3103,7 @@
         <v>45</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F52" s="9">
         <v>43</v>
@@ -3123,7 +3123,7 @@
         <v>46</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>331</v>
+        <v>505</v>
       </c>
       <c r="F53" s="14" t="s">
         <v>260</v>
@@ -3143,7 +3143,7 @@
         <v>47</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>332</v>
+        <v>506</v>
       </c>
       <c r="F54" s="9">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>49</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>333</v>
+        <v>507</v>
       </c>
       <c r="F55" s="9">
         <v>0</v>
@@ -3183,7 +3183,7 @@
         <v>50</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F56" s="9">
         <v>0</v>
@@ -3203,7 +3203,7 @@
         <v>51</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F57" s="9">
         <v>0</v>
@@ -3223,7 +3223,7 @@
         <v>52</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F58" s="9">
         <v>0</v>
@@ -3243,7 +3243,7 @@
         <v>53</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F59" s="9">
         <v>0</v>
@@ -3263,7 +3263,7 @@
         <v>54</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>338</v>
+        <v>508</v>
       </c>
       <c r="F60" s="9">
         <v>0</v>
@@ -3283,7 +3283,7 @@
         <v>55</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>339</v>
+        <v>509</v>
       </c>
       <c r="F61" s="9">
         <v>54</v>
@@ -3303,7 +3303,7 @@
         <v>56</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F62" s="9">
         <v>56</v>
@@ -3323,7 +3323,7 @@
         <v>277</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="F63" s="9">
         <v>58</v>
@@ -3343,7 +3343,7 @@
         <v>57</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="F64" s="9">
         <v>60</v>
@@ -3363,7 +3363,7 @@
         <v>58</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F65" s="9">
         <v>60</v>
@@ -3383,7 +3383,7 @@
         <v>59</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>261</v>
@@ -3403,7 +3403,7 @@
         <v>225</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="F67" s="14">
         <v>57</v>
@@ -3423,7 +3423,7 @@
         <v>60</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>345</v>
+        <v>510</v>
       </c>
       <c r="F68" s="9">
         <v>0</v>
@@ -3443,7 +3443,7 @@
         <v>61</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="F69" s="9">
         <v>62</v>
@@ -3463,7 +3463,7 @@
         <v>62</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F70" s="9">
         <v>0</v>
@@ -3483,7 +3483,7 @@
         <v>63</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="F71" s="9">
         <v>65</v>
@@ -3503,7 +3503,7 @@
         <v>233</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="F72" s="9">
         <v>0</v>
@@ -3523,7 +3523,7 @@
         <v>240</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="F73" s="9">
         <v>0</v>
@@ -3543,7 +3543,7 @@
         <v>64</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="F74" s="9">
         <v>68</v>
@@ -3563,7 +3563,7 @@
         <v>65</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="F75" s="9">
         <v>68</v>
@@ -3583,7 +3583,7 @@
         <v>66</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="F76" s="9">
         <v>68</v>
@@ -3603,7 +3603,7 @@
         <v>67</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="F77" s="9">
         <v>59</v>
@@ -3623,7 +3623,7 @@
         <v>68</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="F78" s="9">
         <v>70</v>
@@ -3643,7 +3643,7 @@
         <v>69</v>
       </c>
       <c r="E79" s="17" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="F79" s="9">
         <v>70</v>
@@ -3663,7 +3663,7 @@
         <v>70</v>
       </c>
       <c r="E80" s="17" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>262</v>
@@ -3683,7 +3683,7 @@
         <v>71</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="F81" s="9">
         <v>0</v>
@@ -3703,7 +3703,7 @@
         <v>72</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="F82" s="9">
         <v>0</v>
@@ -3723,7 +3723,7 @@
         <v>73</v>
       </c>
       <c r="E83" s="17" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="F83" s="9">
         <v>76</v>
@@ -3743,7 +3743,7 @@
         <v>203</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="F84" s="9">
         <v>76</v>
@@ -3763,7 +3763,7 @@
         <v>74</v>
       </c>
       <c r="E85" s="17" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="F85" s="9">
         <v>69</v>
@@ -3783,7 +3783,7 @@
         <v>75</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="F86" s="9">
         <v>69</v>
@@ -3803,7 +3803,7 @@
         <v>76</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="F87" s="9">
         <v>69</v>
@@ -3823,7 +3823,7 @@
         <v>234</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="F88" s="9">
         <v>0</v>
@@ -3843,7 +3843,7 @@
         <v>258</v>
       </c>
       <c r="E89" s="17" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="F89" s="9">
         <v>87</v>
@@ -3863,7 +3863,7 @@
         <v>77</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="F90" s="9">
         <v>87</v>
@@ -3883,7 +3883,7 @@
         <v>242</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>369</v>
+        <v>511</v>
       </c>
       <c r="F91" s="9">
         <v>0</v>
@@ -3903,7 +3903,7 @@
         <v>78</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="F92" s="9">
         <v>88</v>
@@ -3923,7 +3923,7 @@
         <v>79</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="F93" s="9">
         <v>89</v>
@@ -3943,7 +3943,7 @@
         <v>80</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="F94" s="9">
         <v>0</v>
@@ -3963,7 +3963,7 @@
         <v>275</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="F95" s="9">
         <v>0</v>
@@ -3983,7 +3983,7 @@
         <v>81</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="F96" s="9">
         <v>90</v>
@@ -4003,7 +4003,7 @@
         <v>82</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="F97" s="9">
         <v>0</v>
@@ -4023,7 +4023,7 @@
         <v>84</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="F98" s="14" t="s">
         <v>263</v>
@@ -4043,7 +4043,7 @@
         <v>85</v>
       </c>
       <c r="E99" s="17" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="F99" s="14" t="s">
         <v>263</v>
@@ -4063,7 +4063,7 @@
         <v>86</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>263</v>
@@ -4083,7 +4083,7 @@
         <v>248</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="F101" s="14" t="s">
         <v>264</v>
@@ -4103,7 +4103,7 @@
         <v>87</v>
       </c>
       <c r="E102" s="17" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="F102" s="14" t="s">
         <v>265</v>
@@ -4123,7 +4123,7 @@
         <v>88</v>
       </c>
       <c r="E103" s="17" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="F103" s="14" t="s">
         <v>265</v>
@@ -4143,7 +4143,7 @@
         <v>89</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="F104" s="14">
         <v>96</v>
@@ -4163,7 +4163,7 @@
         <v>215</v>
       </c>
       <c r="E105" s="16" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="F105" s="14">
         <v>0</v>
@@ -4183,7 +4183,7 @@
         <v>91</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="F106" s="14">
         <v>0</v>
@@ -4203,7 +4203,7 @@
         <v>92</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="F107" s="14">
         <v>104</v>
@@ -4223,7 +4223,7 @@
         <v>219</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>386</v>
+        <v>512</v>
       </c>
       <c r="F108" s="14">
         <v>105</v>
@@ -4243,7 +4243,7 @@
         <v>218</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="F109" s="14">
         <v>105</v>
@@ -4263,7 +4263,7 @@
         <v>93</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="F110" s="14">
         <v>106</v>
@@ -4283,7 +4283,7 @@
         <v>94</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="F111" s="19">
         <v>107108</v>
@@ -4303,7 +4303,7 @@
         <v>95</v>
       </c>
       <c r="E112" s="17" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="F112" s="14">
         <v>0</v>
@@ -4323,7 +4323,7 @@
         <v>250</v>
       </c>
       <c r="E113" s="17" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="F113" s="14">
         <v>110</v>
@@ -4343,7 +4343,7 @@
         <v>249</v>
       </c>
       <c r="E114" s="17" t="s">
-        <v>392</v>
+        <v>513</v>
       </c>
       <c r="F114" s="14">
         <v>111</v>
@@ -4363,7 +4363,7 @@
         <v>96</v>
       </c>
       <c r="E115" s="17" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="F115" s="14">
         <v>0</v>
@@ -4383,7 +4383,7 @@
         <v>97</v>
       </c>
       <c r="E116" s="17" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="F116" s="14">
         <v>112</v>
@@ -4403,7 +4403,7 @@
         <v>98</v>
       </c>
       <c r="E117" s="17" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="F117" s="14">
         <v>113</v>
@@ -4423,7 +4423,7 @@
         <v>99</v>
       </c>
       <c r="E118" s="17" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="F118" s="14">
         <v>0</v>
@@ -4443,7 +4443,7 @@
         <v>100</v>
       </c>
       <c r="E119" s="17" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="F119" s="14">
         <v>0</v>
@@ -4463,7 +4463,7 @@
         <v>101</v>
       </c>
       <c r="E120" s="17" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="F120" s="14">
         <v>0</v>
@@ -4483,7 +4483,7 @@
         <v>103</v>
       </c>
       <c r="E121" s="17" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="F121" s="14">
         <v>0</v>
@@ -4503,7 +4503,7 @@
         <v>104</v>
       </c>
       <c r="E122" s="17" t="s">
-        <v>400</v>
+        <v>514</v>
       </c>
       <c r="F122" s="14">
         <v>0</v>
@@ -4523,7 +4523,7 @@
         <v>105</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="F123" s="14">
         <v>0</v>
@@ -4543,7 +4543,7 @@
         <v>106</v>
       </c>
       <c r="E124" s="17" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="F124" s="14">
         <v>120</v>
@@ -4563,7 +4563,7 @@
         <v>107</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="F125" s="14">
         <v>121</v>
@@ -4583,7 +4583,7 @@
         <v>108</v>
       </c>
       <c r="E126" s="17" t="s">
-        <v>404</v>
+        <v>515</v>
       </c>
       <c r="F126" s="14">
         <v>123</v>
@@ -4603,7 +4603,7 @@
         <v>109</v>
       </c>
       <c r="E127" s="17" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="F127" s="14">
         <v>124</v>
@@ -4623,7 +4623,7 @@
         <v>266</v>
       </c>
       <c r="E128" s="17" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="F128" s="14">
         <v>122</v>
@@ -4643,7 +4643,7 @@
         <v>235</v>
       </c>
       <c r="E129" s="17" t="s">
-        <v>407</v>
+        <v>516</v>
       </c>
       <c r="F129" s="14">
         <v>0</v>
@@ -4663,7 +4663,7 @@
         <v>267</v>
       </c>
       <c r="E130" s="17" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="F130" s="14">
         <v>125</v>
@@ -4683,7 +4683,7 @@
         <v>268</v>
       </c>
       <c r="E131" s="17" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="F131" s="14">
         <v>0</v>
@@ -4703,7 +4703,7 @@
         <v>110</v>
       </c>
       <c r="E132" s="17" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="F132" s="14">
         <v>126</v>
@@ -4723,7 +4723,7 @@
         <v>111</v>
       </c>
       <c r="E133" s="17" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="F133" s="14">
         <v>127</v>
@@ -4743,7 +4743,7 @@
         <v>112</v>
       </c>
       <c r="E134" s="17" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="F134" s="14">
         <v>0</v>
@@ -4763,7 +4763,7 @@
         <v>269</v>
       </c>
       <c r="E135" s="17" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="F135" s="14">
         <v>129</v>
@@ -4783,7 +4783,7 @@
         <v>113</v>
       </c>
       <c r="E136" s="17" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="F136" s="14">
         <v>0</v>
@@ -4803,7 +4803,7 @@
         <v>270</v>
       </c>
       <c r="E137" s="17" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="F137" s="14">
         <v>0</v>
@@ -4823,7 +4823,7 @@
         <v>271</v>
       </c>
       <c r="E138" s="17" t="s">
-        <v>416</v>
+        <v>517</v>
       </c>
       <c r="F138" s="14">
         <v>0</v>
@@ -4843,7 +4843,7 @@
         <v>272</v>
       </c>
       <c r="E139" s="17" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="F139" s="14">
         <v>0</v>
@@ -4863,7 +4863,7 @@
         <v>114</v>
       </c>
       <c r="E140" s="17" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="F140" s="14">
         <v>137</v>
@@ -4883,7 +4883,7 @@
         <v>273</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
       <c r="F141" s="14">
         <v>138</v>
@@ -4903,7 +4903,7 @@
         <v>274</v>
       </c>
       <c r="E142" s="17" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="F142" s="14">
         <v>0</v>
@@ -4923,7 +4923,7 @@
         <v>116</v>
       </c>
       <c r="E143" s="17" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="F143" s="14">
         <v>139</v>
@@ -4943,7 +4943,7 @@
         <v>251</v>
       </c>
       <c r="E144" s="17" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="F144" s="14">
         <v>0</v>
@@ -4963,7 +4963,7 @@
         <v>252</v>
       </c>
       <c r="E145" s="17" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F145" s="14">
         <v>141</v>
@@ -4983,7 +4983,7 @@
         <v>117</v>
       </c>
       <c r="E146" s="17" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="F146" s="14">
         <v>143</v>
@@ -5003,7 +5003,7 @@
         <v>118</v>
       </c>
       <c r="E147" s="17" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="F147" s="14">
         <v>145</v>
@@ -5023,7 +5023,7 @@
         <v>119</v>
       </c>
       <c r="E148" s="17" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="F148" s="14">
         <v>136</v>
@@ -5043,7 +5043,7 @@
         <v>120</v>
       </c>
       <c r="E149" s="17" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="F149" s="14">
         <v>146</v>
@@ -5063,7 +5063,7 @@
         <v>121</v>
       </c>
       <c r="E150" s="17" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="F150" s="14">
         <v>147</v>
@@ -5083,7 +5083,7 @@
         <v>221</v>
       </c>
       <c r="E151" s="17" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="F151" s="14">
         <v>0</v>
@@ -5103,7 +5103,7 @@
         <v>222</v>
       </c>
       <c r="E152" s="17" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="F152" s="14">
         <v>0</v>
@@ -5123,7 +5123,7 @@
         <v>123</v>
       </c>
       <c r="E153" s="17" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="F153" s="14">
         <v>0</v>
@@ -5143,7 +5143,7 @@
         <v>223</v>
       </c>
       <c r="E154" s="17" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="F154" s="14">
         <v>0</v>
@@ -5163,7 +5163,7 @@
         <v>236</v>
       </c>
       <c r="E155" s="17" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="F155" s="14">
         <v>151</v>
@@ -5183,7 +5183,7 @@
         <v>241</v>
       </c>
       <c r="E156" s="17" t="s">
-        <v>434</v>
+        <v>518</v>
       </c>
       <c r="F156" s="14">
         <v>152</v>
@@ -5203,7 +5203,7 @@
         <v>253</v>
       </c>
       <c r="E157" s="17" t="s">
-        <v>435</v>
+        <v>519</v>
       </c>
       <c r="F157" s="14">
         <v>0</v>
@@ -5223,7 +5223,7 @@
         <v>238</v>
       </c>
       <c r="E158" s="17" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
       <c r="F158" s="14">
         <v>154</v>
@@ -5243,7 +5243,7 @@
         <v>254</v>
       </c>
       <c r="E159" s="17" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="F159" s="14">
         <v>155</v>
@@ -5263,7 +5263,7 @@
         <v>255</v>
       </c>
       <c r="E160" s="17" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="F160" s="19">
         <v>156157</v>
@@ -5283,7 +5283,7 @@
         <v>127</v>
       </c>
       <c r="E161" s="17" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="F161" s="14">
         <v>159</v>
@@ -5303,7 +5303,7 @@
         <v>259</v>
       </c>
       <c r="E162" s="17" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="F162" s="14">
         <v>160</v>
@@ -5323,7 +5323,7 @@
         <v>124</v>
       </c>
       <c r="E163" s="17" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="F163" s="14">
         <v>160</v>
@@ -5343,7 +5343,7 @@
         <v>226</v>
       </c>
       <c r="E164" s="17" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="F164" s="14">
         <v>0</v>
@@ -5363,7 +5363,7 @@
         <v>126</v>
       </c>
       <c r="E165" s="17" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
       <c r="F165" s="19">
         <v>161</v>
@@ -5383,7 +5383,7 @@
         <v>125</v>
       </c>
       <c r="E166" s="17" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
       <c r="F166" s="19">
         <v>162</v>
@@ -5403,7 +5403,7 @@
         <v>128</v>
       </c>
       <c r="E167" s="17" t="s">
-        <v>445</v>
+        <v>426</v>
       </c>
       <c r="F167" s="19">
         <v>161</v>
@@ -5423,7 +5423,7 @@
         <v>129</v>
       </c>
       <c r="E168" s="17" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="F168" s="14">
         <v>163</v>
@@ -5443,7 +5443,7 @@
         <v>239</v>
       </c>
       <c r="E169" s="17" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="F169" s="14">
         <v>0</v>
@@ -5463,7 +5463,7 @@
         <v>276</v>
       </c>
       <c r="E170" s="17" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="F170" s="14">
         <v>0</v>
@@ -5483,7 +5483,7 @@
         <v>53</v>
       </c>
       <c r="E171" s="17" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="F171" s="14">
         <v>0</v>
@@ -5503,7 +5503,7 @@
         <v>130</v>
       </c>
       <c r="E172" s="17" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="F172" s="14">
         <v>0</v>
@@ -5523,7 +5523,7 @@
         <v>131</v>
       </c>
       <c r="E173" s="17" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="F173" s="14">
         <v>0</v>
@@ -5543,7 +5543,7 @@
         <v>227</v>
       </c>
       <c r="E174" s="17" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="F174" s="14">
         <v>0</v>
@@ -5563,7 +5563,7 @@
         <v>132</v>
       </c>
       <c r="E175" s="16" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="F175" s="14">
         <v>0</v>
@@ -5583,7 +5583,7 @@
         <v>133</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="F176" s="14">
         <v>0</v>
@@ -5603,7 +5603,7 @@
         <v>135</v>
       </c>
       <c r="E177" s="16" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="F177" s="19">
         <v>171172173</v>
@@ -5623,7 +5623,7 @@
         <v>136</v>
       </c>
       <c r="E178" s="16" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
       <c r="F178" s="19">
         <v>171172173</v>
@@ -5643,7 +5643,7 @@
         <v>137</v>
       </c>
       <c r="E179" s="16" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="F179" s="14">
         <v>174</v>
@@ -5663,7 +5663,7 @@
         <v>138</v>
       </c>
       <c r="E180" s="16" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
       <c r="F180" s="19">
         <v>177178</v>
@@ -5683,7 +5683,7 @@
         <v>139</v>
       </c>
       <c r="E181" s="16" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="F181" s="19">
         <v>177178</v>
@@ -5703,7 +5703,7 @@
         <v>140</v>
       </c>
       <c r="E182" s="16" t="s">
-        <v>472</v>
+        <v>453</v>
       </c>
       <c r="F182" s="19">
         <v>177178</v>
@@ -5723,7 +5723,7 @@
         <v>141</v>
       </c>
       <c r="E183" s="16" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
       <c r="F183" s="19">
         <v>177178</v>
@@ -5743,7 +5743,7 @@
         <v>142</v>
       </c>
       <c r="E184" s="16" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="F184" s="19">
         <v>177178</v>
@@ -5763,7 +5763,7 @@
         <v>143</v>
       </c>
       <c r="E185" s="16" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="F185" s="14">
         <v>0</v>
@@ -5783,7 +5783,7 @@
         <v>144</v>
       </c>
       <c r="E186" s="16" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="F186" s="14">
         <v>179</v>
@@ -5803,7 +5803,7 @@
         <v>145</v>
       </c>
       <c r="E187" s="16" t="s">
-        <v>468</v>
+        <v>449</v>
       </c>
       <c r="F187" s="14">
         <v>0</v>
@@ -5823,7 +5823,7 @@
         <v>146</v>
       </c>
       <c r="E188" s="16" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
       <c r="F188" s="19">
         <v>180181182183184</v>
@@ -5843,7 +5843,7 @@
         <v>147</v>
       </c>
       <c r="E189" s="16" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="F189" s="19">
         <v>180181182183184</v>
@@ -5863,7 +5863,7 @@
         <v>148</v>
       </c>
       <c r="E190" s="16" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="F190" s="19">
         <v>180181182183184</v>
@@ -5883,7 +5883,7 @@
         <v>149</v>
       </c>
       <c r="E191" s="16" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
       <c r="F191" s="14">
         <v>0</v>
@@ -5903,7 +5903,7 @@
         <v>150</v>
       </c>
       <c r="E192" s="16" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="F192" s="14">
         <v>0</v>
@@ -5923,7 +5923,7 @@
         <v>151</v>
       </c>
       <c r="E193" s="16" t="s">
-        <v>470</v>
+        <v>451</v>
       </c>
       <c r="F193" s="14">
         <v>0</v>
@@ -5943,7 +5943,7 @@
         <v>152</v>
       </c>
       <c r="E194" s="16" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
       <c r="F194" s="14">
         <v>186</v>
@@ -5963,7 +5963,7 @@
         <v>153</v>
       </c>
       <c r="E195" s="16" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="F195" s="14">
         <v>191</v>
@@ -5983,7 +5983,7 @@
         <v>278</v>
       </c>
       <c r="E196" s="16" t="s">
-        <v>474</v>
+        <v>455</v>
       </c>
       <c r="F196" s="14">
         <v>0</v>
@@ -6003,7 +6003,7 @@
         <v>155</v>
       </c>
       <c r="E197" s="16" t="s">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="F197" s="14">
         <v>0</v>
@@ -6023,7 +6023,7 @@
         <v>156</v>
       </c>
       <c r="E198" s="16" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="F198" s="14">
         <v>0</v>
@@ -6043,7 +6043,7 @@
         <v>157</v>
       </c>
       <c r="E199" s="16" t="s">
-        <v>477</v>
+        <v>458</v>
       </c>
       <c r="F199" s="14">
         <v>0</v>
@@ -6063,7 +6063,7 @@
         <v>158</v>
       </c>
       <c r="E200" s="16" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
       <c r="F200" s="14">
         <v>0</v>
@@ -6083,7 +6083,7 @@
         <v>159</v>
       </c>
       <c r="E201" s="16" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="F201" s="14">
         <v>0</v>
@@ -6103,7 +6103,7 @@
         <v>160</v>
       </c>
       <c r="E202" s="16" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
       <c r="F202" s="14">
         <v>0</v>
@@ -6123,7 +6123,7 @@
         <v>161</v>
       </c>
       <c r="E203" s="17" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="F203" s="14">
         <v>0</v>
@@ -6143,7 +6143,7 @@
         <v>237</v>
       </c>
       <c r="E204" s="17" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="F204" s="14">
         <v>197</v>
@@ -6163,7 +6163,7 @@
         <v>256</v>
       </c>
       <c r="E205" s="17" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
       <c r="F205" s="19">
         <v>198199200201</v>
@@ -6183,7 +6183,7 @@
         <v>257</v>
       </c>
       <c r="E206" s="17" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
       <c r="F206" s="19">
         <v>198199200201</v>
@@ -6203,7 +6203,7 @@
         <v>162</v>
       </c>
       <c r="E207" s="17" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="F207" s="19">
         <v>198199200201</v>
@@ -6223,7 +6223,7 @@
         <v>163</v>
       </c>
       <c r="E208" s="17" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="F208" s="19">
         <v>198199200201</v>
@@ -6243,7 +6243,7 @@
         <v>164</v>
       </c>
       <c r="E209" s="17" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="F209" s="14">
         <v>0</v>
@@ -6263,7 +6263,7 @@
         <v>228</v>
       </c>
       <c r="E210" s="17" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="F210" s="14">
         <v>0</v>
@@ -6283,7 +6283,7 @@
         <v>165</v>
       </c>
       <c r="E211" s="17" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="F211" s="14">
         <v>204</v>
@@ -6303,7 +6303,7 @@
         <v>166</v>
       </c>
       <c r="E212" s="17" t="s">
-        <v>490</v>
+        <v>470</v>
       </c>
       <c r="F212" s="19">
         <v>205206207208</v>
@@ -6323,7 +6323,7 @@
         <v>167</v>
       </c>
       <c r="E213" s="17" t="s">
-        <v>492</v>
+        <v>472</v>
       </c>
       <c r="F213" s="14">
         <v>0</v>
@@ -6343,7 +6343,7 @@
         <v>168</v>
       </c>
       <c r="E214" s="17" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="F214" s="14">
         <v>202</v>
@@ -6363,7 +6363,7 @@
         <v>169</v>
       </c>
       <c r="E215" s="17" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="F215" s="14">
         <v>209</v>
@@ -6383,7 +6383,7 @@
         <v>170</v>
       </c>
       <c r="E216" s="17" t="s">
-        <v>494</v>
+        <v>474</v>
       </c>
       <c r="F216" s="14">
         <v>211</v>
@@ -6403,7 +6403,7 @@
         <v>171</v>
       </c>
       <c r="E217" s="17" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
       <c r="F217" s="14">
         <v>211</v>
@@ -6423,7 +6423,7 @@
         <v>172</v>
       </c>
       <c r="E218" s="17" t="s">
-        <v>496</v>
+        <v>476</v>
       </c>
       <c r="F218" s="19">
         <v>212213</v>
@@ -6443,7 +6443,7 @@
         <v>216</v>
       </c>
       <c r="E219" s="17" t="s">
-        <v>497</v>
+        <v>521</v>
       </c>
       <c r="F219" s="19">
         <v>212213</v>
@@ -6463,7 +6463,7 @@
         <v>173</v>
       </c>
       <c r="E220" s="17" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="F220" s="14">
         <v>0</v>
@@ -6483,7 +6483,7 @@
         <v>174</v>
       </c>
       <c r="E221" s="17" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="F221" s="14">
         <v>215</v>
@@ -6503,7 +6503,7 @@
         <v>175</v>
       </c>
       <c r="E222" s="17" t="s">
-        <v>500</v>
+        <v>522</v>
       </c>
       <c r="F222" s="19">
         <v>216217</v>
@@ -6523,7 +6523,7 @@
         <v>176</v>
       </c>
       <c r="E223" s="17" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
       <c r="F223" s="19">
         <v>216217</v>
@@ -6543,7 +6543,7 @@
         <v>177</v>
       </c>
       <c r="E224" s="17" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
       <c r="F224" s="19">
         <v>216217</v>
@@ -6563,7 +6563,7 @@
         <v>217</v>
       </c>
       <c r="E225" s="17" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
       <c r="F225" s="19">
         <v>218219</v>
@@ -6583,7 +6583,7 @@
         <v>178</v>
       </c>
       <c r="E226" s="17" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
       <c r="F226" s="19">
         <v>218219</v>
@@ -6603,7 +6603,7 @@
         <v>179</v>
       </c>
       <c r="E227" s="17" t="s">
-        <v>505</v>
+        <v>483</v>
       </c>
       <c r="F227" s="19">
         <v>218219</v>
@@ -6623,7 +6623,7 @@
         <v>180</v>
       </c>
       <c r="E228" s="17" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="F228" s="14">
         <v>214</v>
@@ -6643,7 +6643,7 @@
         <v>181</v>
       </c>
       <c r="E229" s="17" t="s">
-        <v>507</v>
+        <v>485</v>
       </c>
       <c r="F229" s="14">
         <v>0</v>
@@ -6663,7 +6663,7 @@
         <v>182</v>
       </c>
       <c r="E230" s="17" t="s">
-        <v>508</v>
+        <v>486</v>
       </c>
       <c r="F230" s="14">
         <v>221</v>
@@ -6683,7 +6683,7 @@
         <v>184</v>
       </c>
       <c r="E231" s="17" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="F231" s="14">
         <v>0</v>
@@ -6703,7 +6703,7 @@
         <v>185</v>
       </c>
       <c r="E232" s="17" t="s">
-        <v>510</v>
+        <v>487</v>
       </c>
       <c r="F232" s="14">
         <v>0</v>
@@ -6723,7 +6723,7 @@
         <v>186</v>
       </c>
       <c r="E233" s="17" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="F233" s="14">
         <v>0</v>
@@ -6743,7 +6743,7 @@
         <v>187</v>
       </c>
       <c r="E234" s="17" t="s">
-        <v>512</v>
+        <v>489</v>
       </c>
       <c r="F234" s="14">
         <v>0</v>
@@ -6763,7 +6763,7 @@
         <v>188</v>
       </c>
       <c r="E235" s="17" t="s">
-        <v>513</v>
+        <v>490</v>
       </c>
       <c r="F235" s="19">
         <v>231232</v>
@@ -6783,7 +6783,7 @@
         <v>189</v>
       </c>
       <c r="E236" s="17" t="s">
-        <v>514</v>
+        <v>491</v>
       </c>
       <c r="F236" s="14">
         <v>234</v>
@@ -6803,7 +6803,7 @@
         <v>190</v>
       </c>
       <c r="E237" s="17" t="s">
-        <v>515</v>
+        <v>492</v>
       </c>
       <c r="F237" s="14">
         <v>0</v>
@@ -6823,7 +6823,7 @@
         <v>191</v>
       </c>
       <c r="E238" s="17" t="s">
-        <v>516</v>
+        <v>493</v>
       </c>
       <c r="F238" s="14">
         <v>232</v>
@@ -6843,7 +6843,7 @@
         <v>192</v>
       </c>
       <c r="E239" s="17" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="F239" s="14">
         <v>235</v>
@@ -6863,7 +6863,7 @@
         <v>193</v>
       </c>
       <c r="E240" s="17" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
       <c r="F240" s="14">
         <v>235</v>
@@ -6883,7 +6883,7 @@
         <v>194</v>
       </c>
       <c r="E241" s="17" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="F241" s="14">
         <v>237</v>
@@ -6903,7 +6903,7 @@
         <v>195</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>520</v>
+        <v>495</v>
       </c>
       <c r="F242" s="14">
         <v>0</v>
@@ -6923,7 +6923,7 @@
         <v>196</v>
       </c>
       <c r="E243" s="16" t="s">
-        <v>521</v>
+        <v>496</v>
       </c>
       <c r="F243" s="19">
         <v>239240</v>
@@ -6943,7 +6943,7 @@
         <v>197</v>
       </c>
       <c r="E244" s="16" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="F244" s="19">
         <v>239240</v>
@@ -6963,7 +6963,7 @@
         <v>198</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>523</v>
+        <v>497</v>
       </c>
       <c r="F245" s="14">
         <v>242</v>
@@ -6983,7 +6983,7 @@
         <v>199</v>
       </c>
       <c r="E246" s="16" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="F246" s="19">
         <v>243244</v>
@@ -7003,7 +7003,7 @@
         <v>200</v>
       </c>
       <c r="E247" s="16" t="s">
-        <v>524</v>
+        <v>498</v>
       </c>
       <c r="F247" s="19">
         <v>243244</v>
@@ -7023,7 +7023,7 @@
         <v>201</v>
       </c>
       <c r="E248" s="16" t="s">
-        <v>525</v>
+        <v>499</v>
       </c>
       <c r="F248" s="19">
         <v>243244</v>
@@ -7043,7 +7043,7 @@
         <v>202</v>
       </c>
       <c r="E249" s="3" t="s">
-        <v>526</v>
+        <v>500</v>
       </c>
       <c r="F249" s="14">
         <v>245</v>

</xml_diff>

<commit_message>
Brain: Adding more details to the acceptance criteria for some of the continuous integration capabilities
</commit_message>
<xml_diff>
--- a/Continuum in Excel map v 2.xlsx
+++ b/Continuum in Excel map v 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A228900\Documents\Projects\brain-edit\continuum-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A228900\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1019,18 +1019,12 @@
     <t>All the testing performed are manual, predominantly exploratory type tests. Team needs to start implementing automated tests.</t>
   </si>
   <si>
-    <t>There's a script to build the application and this process is automated. There are also tests run as part of the build process.</t>
-  </si>
-  <si>
     <t>There are some test cases but not all of them have been automated. The test coverage is greater than zero but less than 50%. Team needs to improve on the test coverage and move it towards 50%. Team also needs to automate the test cases they have (this will need to be prioritised in the backlog as well and some slack put in the system to cater for this)</t>
   </si>
   <si>
     <t>The team checks in code every day to the version management tool. Team still works on several long-lived branches but the code is checked in at least once a day. Team needs to start moving towards very short lived branches</t>
   </si>
   <si>
-    <t>All the artefacts such as packages, build scripts, etc are checked in to the version management system. Every new team member can check out the source code and build the application from the version management system.</t>
-  </si>
-  <si>
     <t>Builds are triggered by simple click of a button on the continuous integration management tool.</t>
   </si>
   <si>
@@ -1065,9 +1059,6 @@
   </si>
   <si>
     <t>The build and deployment processes are automated as much as the constraints allow. This should be automated preferably all the way to production, however, in some organisations this may not be possible. The steps to production exists and can be triggered manually on receiving the requisite approvals.</t>
-  </si>
-  <si>
-    <t>The team has a build pipeline that extends directly to production. Artefacts and code can be promoted through various environments all the way to production.</t>
   </si>
   <si>
     <t>To speed up the regression tests feedback, the teams have parallelized the tests suites across multiple machines.</t>
@@ -1644,6 +1635,15 @@
       </rPr>
       <t xml:space="preserve"> have been identified</t>
     </r>
+  </si>
+  <si>
+    <t>There's a script to build the application and this process is automated. There are also tests run as part of the build process. The build of the application is performed via a simple command</t>
+  </si>
+  <si>
+    <t>All the artefacts such as packages, build scripts, etc are checked in to the version management system. Every new team member can check out the source code and build the application from the version management system. Artefacts like database schemas, deployment scripts etc</t>
+  </si>
+  <si>
+    <t>The team has a build pipeline that extends directly to production. Artefacts and code can be promoted through various environments all the way to production. A defect in production can be fixed within minutes rather than hours/days/weeks. If no deployment to production the team is deploying to an environment that is very similar to the production environment.</t>
   </si>
 </sst>
 </file>
@@ -1739,7 +1739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1799,6 +1799,12 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2083,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197:XFD230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2131,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F2" s="9">
         <v>0</v>
@@ -2191,7 +2197,7 @@
         <v>231</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F5" s="9">
         <v>1</v>
@@ -2371,7 +2377,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F14" s="9">
         <v>9</v>
@@ -2608,7 +2614,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>299</v>
@@ -2628,7 +2634,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>300</v>
@@ -2811,7 +2817,7 @@
         <v>209</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F36" s="9">
         <v>29</v>
@@ -3151,7 +3157,7 @@
         <v>45</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F53" s="14" t="s">
         <v>258</v>
@@ -3171,294 +3177,294 @@
         <v>46</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F54" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="22" t="s">
         <v>219</v>
       </c>
       <c r="C55" s="10">
         <v>54</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E55" s="16" t="s">
-        <v>505</v>
+      <c r="E55" s="17" t="s">
+        <v>502</v>
       </c>
       <c r="F55" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="10">
         <v>55</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="17" t="s">
         <v>325</v>
       </c>
       <c r="F56" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="10">
         <v>56</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="17" t="s">
         <v>326</v>
       </c>
       <c r="F57" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
+    <row r="58" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A58" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="10">
         <v>57</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="17" t="s">
         <v>327</v>
       </c>
       <c r="F58" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
+    <row r="59" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="10">
         <v>58</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="17" t="s">
         <v>328</v>
       </c>
       <c r="F59" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
+    <row r="60" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="10">
         <v>59</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E60" s="16" t="s">
-        <v>506</v>
+      <c r="E60" s="17" t="s">
+        <v>503</v>
       </c>
       <c r="F60" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
+    <row r="61" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="10">
         <v>60</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E61" s="16" t="s">
-        <v>507</v>
+      <c r="E61" s="17" t="s">
+        <v>504</v>
       </c>
       <c r="F61" s="9">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
+    <row r="62" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="10">
         <v>61</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>329</v>
+        <v>524</v>
       </c>
       <c r="F62" s="9">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
+    <row r="63" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A63" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="10">
         <v>62</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>275</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F63" s="9">
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="6" t="s">
+    <row r="64" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="10">
         <v>63</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>56</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F64" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
+    <row r="65" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="10">
         <v>64</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>57</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>332</v>
+        <v>525</v>
       </c>
       <c r="F65" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
+    <row r="66" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A66" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="10">
         <v>65</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E66" s="16" t="s">
-        <v>336</v>
+      <c r="E66" s="17" t="s">
+        <v>334</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="6" t="s">
+    <row r="67" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="10">
         <v>66</v>
       </c>
       <c r="D67" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F67" s="14">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A68" s="6" t="s">
+    <row r="68" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A68" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="10">
         <v>67</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="16" t="s">
-        <v>508</v>
+      <c r="E68" s="17" t="s">
+        <v>505</v>
       </c>
       <c r="F68" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+    <row r="69" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B69" s="10" t="s">
@@ -3471,14 +3477,14 @@
         <v>60</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F69" s="9">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
+    <row r="70" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B70" s="10" t="s">
@@ -3491,14 +3497,14 @@
         <v>61</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F70" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="6" t="s">
+    <row r="71" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B71" s="10" t="s">
@@ -3511,14 +3517,14 @@
         <v>62</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F71" s="9">
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="6" t="s">
+    <row r="72" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B72" s="10" t="s">
@@ -3531,14 +3537,14 @@
         <v>232</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F72" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
+    <row r="73" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B73" s="10" t="s">
@@ -3551,14 +3557,14 @@
         <v>239</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F73" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+    <row r="74" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B74" s="10" t="s">
@@ -3571,14 +3577,14 @@
         <v>63</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F74" s="9">
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
+    <row r="75" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A75" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B75" s="10" t="s">
@@ -3591,14 +3597,14 @@
         <v>64</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F75" s="9">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
+    <row r="76" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A76" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B76" s="10" t="s">
@@ -3611,14 +3617,14 @@
         <v>65</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F76" s="9">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
+    <row r="77" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B77" s="10" t="s">
@@ -3631,14 +3637,14 @@
         <v>66</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F77" s="9">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A78" s="6" t="s">
+    <row r="78" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A78" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B78" s="10" t="s">
@@ -3651,14 +3657,14 @@
         <v>67</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F78" s="9">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
+    <row r="79" spans="1:6" s="10" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A79" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B79" s="10" t="s">
@@ -3671,14 +3677,14 @@
         <v>68</v>
       </c>
       <c r="E79" s="17" t="s">
-        <v>345</v>
+        <v>526</v>
       </c>
       <c r="F79" s="9">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A80" s="6" t="s">
+    <row r="80" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B80" s="10" t="s">
@@ -3691,14 +3697,14 @@
         <v>69</v>
       </c>
       <c r="E80" s="17" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A81" s="6" t="s">
+    <row r="81" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A81" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B81" s="10" t="s">
@@ -3711,14 +3717,14 @@
         <v>70</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F81" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="6" t="s">
+    <row r="82" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B82" s="10" t="s">
@@ -3731,14 +3737,14 @@
         <v>71</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F82" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
+    <row r="83" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B83" s="10" t="s">
@@ -3751,14 +3757,14 @@
         <v>72</v>
       </c>
       <c r="E83" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F83" s="9">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
+    <row r="84" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B84" s="10" t="s">
@@ -3771,14 +3777,14 @@
         <v>202</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F84" s="9">
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="6" t="s">
+    <row r="85" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B85" s="10" t="s">
@@ -3791,14 +3797,14 @@
         <v>73</v>
       </c>
       <c r="E85" s="17" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F85" s="9">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
+    <row r="86" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A86" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B86" s="10" t="s">
@@ -3811,14 +3817,14 @@
         <v>74</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F86" s="9">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A87" s="6" t="s">
+    <row r="87" spans="1:6" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A87" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B87" s="10" t="s">
@@ -3831,7 +3837,7 @@
         <v>75</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F87" s="9">
         <v>69</v>
@@ -3851,7 +3857,7 @@
         <v>233</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F88" s="9">
         <v>0</v>
@@ -3871,7 +3877,7 @@
         <v>256</v>
       </c>
       <c r="E89" s="17" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F89" s="9">
         <v>87</v>
@@ -3891,7 +3897,7 @@
         <v>76</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F90" s="9">
         <v>87</v>
@@ -3911,7 +3917,7 @@
         <v>241</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F91" s="9">
         <v>0</v>
@@ -3931,7 +3937,7 @@
         <v>77</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F92" s="9">
         <v>88</v>
@@ -3951,7 +3957,7 @@
         <v>78</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F93" s="9">
         <v>89</v>
@@ -3971,7 +3977,7 @@
         <v>79</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F94" s="9">
         <v>0</v>
@@ -3991,7 +3997,7 @@
         <v>273</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F95" s="9">
         <v>0</v>
@@ -4011,7 +4017,7 @@
         <v>80</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F96" s="9">
         <v>90</v>
@@ -4031,7 +4037,7 @@
         <v>81</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F97" s="9">
         <v>0</v>
@@ -4051,7 +4057,7 @@
         <v>83</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F98" s="14" t="s">
         <v>261</v>
@@ -4071,7 +4077,7 @@
         <v>84</v>
       </c>
       <c r="E99" s="17" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F99" s="14" t="s">
         <v>261</v>
@@ -4091,7 +4097,7 @@
         <v>85</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>261</v>
@@ -4111,7 +4117,7 @@
         <v>246</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F101" s="14" t="s">
         <v>262</v>
@@ -4131,7 +4137,7 @@
         <v>86</v>
       </c>
       <c r="E102" s="17" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F102" s="14" t="s">
         <v>263</v>
@@ -4151,7 +4157,7 @@
         <v>87</v>
       </c>
       <c r="E103" s="17" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F103" s="14" t="s">
         <v>263</v>
@@ -4171,7 +4177,7 @@
         <v>88</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F104" s="14">
         <v>96</v>
@@ -4191,7 +4197,7 @@
         <v>214</v>
       </c>
       <c r="E105" s="16" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F105" s="14">
         <v>0</v>
@@ -4211,7 +4217,7 @@
         <v>90</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F106" s="14">
         <v>0</v>
@@ -4231,7 +4237,7 @@
         <v>91</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F107" s="14">
         <v>104</v>
@@ -4251,7 +4257,7 @@
         <v>218</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F108" s="14">
         <v>105</v>
@@ -4271,7 +4277,7 @@
         <v>217</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F109" s="14">
         <v>105</v>
@@ -4291,7 +4297,7 @@
         <v>92</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F110" s="14">
         <v>106</v>
@@ -4311,7 +4317,7 @@
         <v>93</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F111" s="19">
         <v>107108</v>
@@ -4331,7 +4337,7 @@
         <v>94</v>
       </c>
       <c r="E112" s="17" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F112" s="14">
         <v>0</v>
@@ -4351,7 +4357,7 @@
         <v>248</v>
       </c>
       <c r="E113" s="17" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F113" s="14">
         <v>110</v>
@@ -4371,7 +4377,7 @@
         <v>247</v>
       </c>
       <c r="E114" s="17" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F114" s="14">
         <v>111</v>
@@ -4391,7 +4397,7 @@
         <v>95</v>
       </c>
       <c r="E115" s="17" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F115" s="14">
         <v>0</v>
@@ -4411,7 +4417,7 @@
         <v>96</v>
       </c>
       <c r="E116" s="17" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F116" s="14">
         <v>112</v>
@@ -4431,7 +4437,7 @@
         <v>97</v>
       </c>
       <c r="E117" s="17" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F117" s="14">
         <v>113</v>
@@ -4451,7 +4457,7 @@
         <v>98</v>
       </c>
       <c r="E118" s="17" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F118" s="14">
         <v>0</v>
@@ -4471,7 +4477,7 @@
         <v>99</v>
       </c>
       <c r="E119" s="17" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F119" s="14">
         <v>0</v>
@@ -4491,7 +4497,7 @@
         <v>100</v>
       </c>
       <c r="E120" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F120" s="14">
         <v>0</v>
@@ -4511,7 +4517,7 @@
         <v>102</v>
       </c>
       <c r="E121" s="17" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F121" s="14">
         <v>0</v>
@@ -4531,7 +4537,7 @@
         <v>103</v>
       </c>
       <c r="E122" s="17" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F122" s="14">
         <v>0</v>
@@ -4551,7 +4557,7 @@
         <v>104</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F123" s="14">
         <v>0</v>
@@ -4571,7 +4577,7 @@
         <v>105</v>
       </c>
       <c r="E124" s="17" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F124" s="14">
         <v>120</v>
@@ -4591,7 +4597,7 @@
         <v>106</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F125" s="14">
         <v>121</v>
@@ -4611,7 +4617,7 @@
         <v>107</v>
       </c>
       <c r="E126" s="17" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F126" s="14">
         <v>123</v>
@@ -4631,7 +4637,7 @@
         <v>108</v>
       </c>
       <c r="E127" s="17" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F127" s="14">
         <v>124</v>
@@ -4651,7 +4657,7 @@
         <v>264</v>
       </c>
       <c r="E128" s="17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F128" s="14">
         <v>122</v>
@@ -4671,7 +4677,7 @@
         <v>234</v>
       </c>
       <c r="E129" s="17" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F129" s="14">
         <v>0</v>
@@ -4691,7 +4697,7 @@
         <v>265</v>
       </c>
       <c r="E130" s="17" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F130" s="14">
         <v>125</v>
@@ -4711,7 +4717,7 @@
         <v>266</v>
       </c>
       <c r="E131" s="17" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F131" s="14">
         <v>0</v>
@@ -4731,7 +4737,7 @@
         <v>109</v>
       </c>
       <c r="E132" s="17" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F132" s="14">
         <v>126</v>
@@ -4751,7 +4757,7 @@
         <v>110</v>
       </c>
       <c r="E133" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F133" s="14">
         <v>127</v>
@@ -4771,7 +4777,7 @@
         <v>111</v>
       </c>
       <c r="E134" s="17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F134" s="14">
         <v>0</v>
@@ -4791,7 +4797,7 @@
         <v>267</v>
       </c>
       <c r="E135" s="17" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F135" s="14">
         <v>129</v>
@@ -4811,7 +4817,7 @@
         <v>112</v>
       </c>
       <c r="E136" s="17" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F136" s="14">
         <v>0</v>
@@ -4831,7 +4837,7 @@
         <v>268</v>
       </c>
       <c r="E137" s="17" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F137" s="14">
         <v>0</v>
@@ -4851,7 +4857,7 @@
         <v>269</v>
       </c>
       <c r="E138" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F138" s="14">
         <v>0</v>
@@ -4871,7 +4877,7 @@
         <v>270</v>
       </c>
       <c r="E139" s="17" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F139" s="14">
         <v>0</v>
@@ -4891,7 +4897,7 @@
         <v>113</v>
       </c>
       <c r="E140" s="17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F140" s="14">
         <v>137</v>
@@ -4911,7 +4917,7 @@
         <v>271</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F141" s="14">
         <v>138</v>
@@ -4931,7 +4937,7 @@
         <v>272</v>
       </c>
       <c r="E142" s="17" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F142" s="14">
         <v>0</v>
@@ -4951,7 +4957,7 @@
         <v>115</v>
       </c>
       <c r="E143" s="17" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F143" s="14">
         <v>139</v>
@@ -4971,7 +4977,7 @@
         <v>249</v>
       </c>
       <c r="E144" s="17" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F144" s="14">
         <v>0</v>
@@ -4991,7 +4997,7 @@
         <v>250</v>
       </c>
       <c r="E145" s="17" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F145" s="14">
         <v>141</v>
@@ -5011,7 +5017,7 @@
         <v>116</v>
       </c>
       <c r="E146" s="17" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F146" s="14">
         <v>143</v>
@@ -5031,7 +5037,7 @@
         <v>117</v>
       </c>
       <c r="E147" s="17" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F147" s="14">
         <v>145</v>
@@ -5051,7 +5057,7 @@
         <v>118</v>
       </c>
       <c r="E148" s="17" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F148" s="14">
         <v>136</v>
@@ -5071,7 +5077,7 @@
         <v>119</v>
       </c>
       <c r="E149" s="17" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F149" s="14">
         <v>146</v>
@@ -5091,7 +5097,7 @@
         <v>120</v>
       </c>
       <c r="E150" s="17" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F150" s="14">
         <v>147</v>
@@ -5111,7 +5117,7 @@
         <v>220</v>
       </c>
       <c r="E151" s="17" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F151" s="14">
         <v>0</v>
@@ -5131,7 +5137,7 @@
         <v>221</v>
       </c>
       <c r="E152" s="17" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F152" s="14">
         <v>0</v>
@@ -5151,7 +5157,7 @@
         <v>122</v>
       </c>
       <c r="E153" s="17" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="F153" s="14">
         <v>0</v>
@@ -5171,7 +5177,7 @@
         <v>222</v>
       </c>
       <c r="E154" s="17" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F154" s="14">
         <v>0</v>
@@ -5191,7 +5197,7 @@
         <v>235</v>
       </c>
       <c r="E155" s="17" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F155" s="14">
         <v>151</v>
@@ -5211,7 +5217,7 @@
         <v>240</v>
       </c>
       <c r="E156" s="17" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F156" s="14">
         <v>152</v>
@@ -5231,7 +5237,7 @@
         <v>251</v>
       </c>
       <c r="E157" s="17" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F157" s="14">
         <v>0</v>
@@ -5251,7 +5257,7 @@
         <v>237</v>
       </c>
       <c r="E158" s="17" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F158" s="14">
         <v>154</v>
@@ -5271,7 +5277,7 @@
         <v>252</v>
       </c>
       <c r="E159" s="17" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F159" s="14">
         <v>155</v>
@@ -5291,7 +5297,7 @@
         <v>253</v>
       </c>
       <c r="E160" s="17" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F160" s="19">
         <v>156157</v>
@@ -5311,7 +5317,7 @@
         <v>126</v>
       </c>
       <c r="E161" s="17" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F161" s="14">
         <v>159</v>
@@ -5331,7 +5337,7 @@
         <v>257</v>
       </c>
       <c r="E162" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F162" s="14">
         <v>160</v>
@@ -5351,7 +5357,7 @@
         <v>123</v>
       </c>
       <c r="E163" s="17" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F163" s="14">
         <v>160</v>
@@ -5371,7 +5377,7 @@
         <v>225</v>
       </c>
       <c r="E164" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F164" s="14">
         <v>0</v>
@@ -5391,7 +5397,7 @@
         <v>125</v>
       </c>
       <c r="E165" s="17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F165" s="19">
         <v>161</v>
@@ -5411,7 +5417,7 @@
         <v>124</v>
       </c>
       <c r="E166" s="17" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F166" s="19">
         <v>162</v>
@@ -5431,7 +5437,7 @@
         <v>127</v>
       </c>
       <c r="E167" s="17" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F167" s="19">
         <v>161</v>
@@ -5451,7 +5457,7 @@
         <v>128</v>
       </c>
       <c r="E168" s="17" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F168" s="14">
         <v>163</v>
@@ -5471,7 +5477,7 @@
         <v>238</v>
       </c>
       <c r="E169" s="17" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F169" s="14">
         <v>0</v>
@@ -5491,7 +5497,7 @@
         <v>274</v>
       </c>
       <c r="E170" s="17" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F170" s="14">
         <v>0</v>
@@ -5511,7 +5517,7 @@
         <v>52</v>
       </c>
       <c r="E171" s="17" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F171" s="14">
         <v>0</v>
@@ -5531,7 +5537,7 @@
         <v>129</v>
       </c>
       <c r="E172" s="17" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F172" s="14">
         <v>0</v>
@@ -5551,7 +5557,7 @@
         <v>130</v>
       </c>
       <c r="E173" s="17" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F173" s="14">
         <v>0</v>
@@ -5571,7 +5577,7 @@
         <v>226</v>
       </c>
       <c r="E174" s="17" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F174" s="14">
         <v>0</v>
@@ -5591,7 +5597,7 @@
         <v>131</v>
       </c>
       <c r="E175" s="16" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="F175" s="14">
         <v>0</v>
@@ -5611,7 +5617,7 @@
         <v>132</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F176" s="14">
         <v>0</v>
@@ -5631,7 +5637,7 @@
         <v>134</v>
       </c>
       <c r="E177" s="16" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F177" s="19">
         <v>171172173</v>
@@ -5651,7 +5657,7 @@
         <v>135</v>
       </c>
       <c r="E178" s="16" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F178" s="19">
         <v>171172173</v>
@@ -5671,7 +5677,7 @@
         <v>136</v>
       </c>
       <c r="E179" s="16" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F179" s="14">
         <v>174</v>
@@ -5691,7 +5697,7 @@
         <v>137</v>
       </c>
       <c r="E180" s="16" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F180" s="19">
         <v>177178</v>
@@ -5711,7 +5717,7 @@
         <v>138</v>
       </c>
       <c r="E181" s="16" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F181" s="19">
         <v>177178</v>
@@ -5731,7 +5737,7 @@
         <v>139</v>
       </c>
       <c r="E182" s="16" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F182" s="19">
         <v>177178</v>
@@ -5751,7 +5757,7 @@
         <v>140</v>
       </c>
       <c r="E183" s="16" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F183" s="19">
         <v>177178</v>
@@ -5771,7 +5777,7 @@
         <v>141</v>
       </c>
       <c r="E184" s="16" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F184" s="19">
         <v>177178</v>
@@ -5791,7 +5797,7 @@
         <v>142</v>
       </c>
       <c r="E185" s="16" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F185" s="14">
         <v>0</v>
@@ -5811,7 +5817,7 @@
         <v>143</v>
       </c>
       <c r="E186" s="16" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F186" s="14">
         <v>179</v>
@@ -5831,7 +5837,7 @@
         <v>144</v>
       </c>
       <c r="E187" s="16" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F187" s="14">
         <v>0</v>
@@ -5851,7 +5857,7 @@
         <v>145</v>
       </c>
       <c r="E188" s="16" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F188" s="19">
         <v>180181182183184</v>
@@ -5871,7 +5877,7 @@
         <v>146</v>
       </c>
       <c r="E189" s="16" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F189" s="19">
         <v>180181182183184</v>
@@ -5891,7 +5897,7 @@
         <v>147</v>
       </c>
       <c r="E190" s="16" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="F190" s="19">
         <v>180181182183184</v>
@@ -5911,7 +5917,7 @@
         <v>148</v>
       </c>
       <c r="E191" s="16" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F191" s="14">
         <v>0</v>
@@ -5931,7 +5937,7 @@
         <v>149</v>
       </c>
       <c r="E192" s="16" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="F192" s="14">
         <v>0</v>
@@ -5951,7 +5957,7 @@
         <v>150</v>
       </c>
       <c r="E193" s="16" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="F193" s="14">
         <v>0</v>
@@ -5971,7 +5977,7 @@
         <v>151</v>
       </c>
       <c r="E194" s="16" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F194" s="14">
         <v>186</v>
@@ -5991,7 +5997,7 @@
         <v>152</v>
       </c>
       <c r="E195" s="16" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F195" s="14">
         <v>191</v>
@@ -6011,137 +6017,137 @@
         <v>276</v>
       </c>
       <c r="E196" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="F196" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A197" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B197" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C197" s="10">
+        <v>197</v>
+      </c>
+      <c r="D197" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E197" s="17" t="s">
+        <v>451</v>
+      </c>
+      <c r="F197" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A198" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B198" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C198" s="10">
+        <v>198</v>
+      </c>
+      <c r="D198" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E198" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="F198" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A199" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B199" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C199" s="10">
+        <v>199</v>
+      </c>
+      <c r="D199" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E199" s="17" t="s">
         <v>453</v>
       </c>
-      <c r="F196" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A197" s="6" t="s">
+      <c r="F199" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A200" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="B200" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C197" s="1">
-        <v>197</v>
-      </c>
-      <c r="D197" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E197" s="16" t="s">
+      <c r="C200" s="10">
+        <v>200</v>
+      </c>
+      <c r="D200" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E200" s="17" t="s">
         <v>454</v>
       </c>
-      <c r="F197" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A198" s="6" t="s">
+      <c r="F200" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A201" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B198" s="1" t="s">
+      <c r="B201" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C198" s="1">
-        <v>198</v>
-      </c>
-      <c r="D198" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E198" s="16" t="s">
+      <c r="C201" s="10">
+        <v>201</v>
+      </c>
+      <c r="D201" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E201" s="17" t="s">
         <v>455</v>
       </c>
-      <c r="F198" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A199" s="6" t="s">
+      <c r="F201" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A202" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B202" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C199" s="1">
-        <v>199</v>
-      </c>
-      <c r="D199" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="E199" s="16" t="s">
+      <c r="C202" s="10">
+        <v>202</v>
+      </c>
+      <c r="D202" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E202" s="17" t="s">
         <v>456</v>
       </c>
-      <c r="F199" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A200" s="6" t="s">
+      <c r="F202" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A203" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C200" s="1">
-        <v>200</v>
-      </c>
-      <c r="D200" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E200" s="16" t="s">
-        <v>457</v>
-      </c>
-      <c r="F200" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A201" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C201" s="1">
-        <v>201</v>
-      </c>
-      <c r="D201" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E201" s="16" t="s">
-        <v>458</v>
-      </c>
-      <c r="F201" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A202" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C202" s="1">
-        <v>202</v>
-      </c>
-      <c r="D202" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="E202" s="16" t="s">
-        <v>459</v>
-      </c>
-      <c r="F202" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A203" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B203" s="1" t="s">
+      <c r="B203" s="10" t="s">
         <v>219</v>
       </c>
       <c r="C203" s="10">
@@ -6151,17 +6157,17 @@
         <v>160</v>
       </c>
       <c r="E203" s="17" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F203" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A204" s="6" t="s">
+    <row r="204" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A204" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B204" s="1" t="s">
+      <c r="B204" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C204" s="10">
@@ -6171,17 +6177,17 @@
         <v>236</v>
       </c>
       <c r="E204" s="17" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="F204" s="14">
         <v>197</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A205" s="6" t="s">
+    <row r="205" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A205" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B205" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C205" s="10">
@@ -6191,17 +6197,17 @@
         <v>254</v>
       </c>
       <c r="E205" s="17" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="F205" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A206" s="6" t="s">
+    <row r="206" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A206" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="B206" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C206" s="10">
@@ -6211,17 +6217,17 @@
         <v>255</v>
       </c>
       <c r="E206" s="17" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F206" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A207" s="6" t="s">
+    <row r="207" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A207" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B207" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C207" s="10">
@@ -6231,17 +6237,17 @@
         <v>161</v>
       </c>
       <c r="E207" s="17" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F207" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A208" s="6" t="s">
+    <row r="208" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A208" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B208" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C208" s="10">
@@ -6251,17 +6257,17 @@
         <v>162</v>
       </c>
       <c r="E208" s="17" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="F208" s="19">
         <v>198199200201</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A209" s="6" t="s">
+    <row r="209" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A209" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="B209" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C209" s="10">
@@ -6271,17 +6277,17 @@
         <v>163</v>
       </c>
       <c r="E209" s="17" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="F209" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A210" s="6" t="s">
+    <row r="210" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="B210" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C210" s="10">
@@ -6291,17 +6297,17 @@
         <v>227</v>
       </c>
       <c r="E210" s="17" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="F210" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A211" s="6" t="s">
+    <row r="211" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A211" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="B211" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C211" s="10">
@@ -6311,17 +6317,17 @@
         <v>164</v>
       </c>
       <c r="E211" s="17" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F211" s="14">
         <v>204</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A212" s="6" t="s">
+    <row r="212" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A212" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B212" s="1" t="s">
+      <c r="B212" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C212" s="10">
@@ -6331,17 +6337,17 @@
         <v>165</v>
       </c>
       <c r="E212" s="17" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="F212" s="19">
         <v>205206207208</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A213" s="6" t="s">
+    <row r="213" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A213" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="B213" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C213" s="10">
@@ -6351,17 +6357,17 @@
         <v>166</v>
       </c>
       <c r="E213" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F213" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A214" s="6" t="s">
+    <row r="214" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A214" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="B214" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C214" s="10">
@@ -6371,17 +6377,17 @@
         <v>167</v>
       </c>
       <c r="E214" s="17" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F214" s="14">
         <v>202</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A215" s="6" t="s">
+    <row r="215" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A215" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B215" s="1" t="s">
+      <c r="B215" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C215" s="10">
@@ -6391,17 +6397,17 @@
         <v>168</v>
       </c>
       <c r="E215" s="17" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F215" s="14">
         <v>209</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A216" s="6" t="s">
+    <row r="216" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A216" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B216" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C216" s="10">
@@ -6411,17 +6417,17 @@
         <v>169</v>
       </c>
       <c r="E216" s="17" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F216" s="14">
         <v>211</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A217" s="6" t="s">
+    <row r="217" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A217" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B217" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C217" s="10">
@@ -6431,17 +6437,17 @@
         <v>170</v>
       </c>
       <c r="E217" s="17" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="F217" s="14">
         <v>211</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A218" s="6" t="s">
+    <row r="218" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A218" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="B218" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C218" s="10">
@@ -6451,17 +6457,17 @@
         <v>171</v>
       </c>
       <c r="E218" s="17" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F218" s="19">
         <v>212213</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A219" s="6" t="s">
+    <row r="219" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A219" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B219" s="1" t="s">
+      <c r="B219" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C219" s="10">
@@ -6471,17 +6477,17 @@
         <v>215</v>
       </c>
       <c r="E219" s="17" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F219" s="19">
         <v>212213</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A220" s="6" t="s">
+    <row r="220" spans="1:6" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A220" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B220" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C220" s="10">
@@ -6491,17 +6497,17 @@
         <v>172</v>
       </c>
       <c r="E220" s="17" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F220" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A221" s="6" t="s">
+    <row r="221" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A221" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B221" s="1" t="s">
+      <c r="B221" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C221" s="10">
@@ -6511,17 +6517,17 @@
         <v>173</v>
       </c>
       <c r="E221" s="17" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="F221" s="14">
         <v>215</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A222" s="6" t="s">
+    <row r="222" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A222" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B222" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C222" s="10">
@@ -6531,17 +6537,17 @@
         <v>174</v>
       </c>
       <c r="E222" s="17" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F222" s="19">
         <v>216217</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="6" t="s">
+    <row r="223" spans="1:6" s="10" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B223" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C223" s="10">
@@ -6551,17 +6557,17 @@
         <v>175</v>
       </c>
       <c r="E223" s="17" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F223" s="19">
         <v>216217</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A224" s="6" t="s">
+    <row r="224" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A224" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B224" s="1" t="s">
+      <c r="B224" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C224" s="10">
@@ -6571,17 +6577,17 @@
         <v>176</v>
       </c>
       <c r="E224" s="17" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="F224" s="19">
         <v>216217</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A225" s="6" t="s">
+    <row r="225" spans="1:6" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A225" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B225" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C225" s="10">
@@ -6591,17 +6597,17 @@
         <v>216</v>
       </c>
       <c r="E225" s="17" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="F225" s="19">
         <v>218219</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A226" s="6" t="s">
+    <row r="226" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A226" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B226" s="1" t="s">
+      <c r="B226" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C226" s="10">
@@ -6611,17 +6617,17 @@
         <v>177</v>
       </c>
       <c r="E226" s="17" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F226" s="19">
         <v>218219</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A227" s="6" t="s">
+    <row r="227" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A227" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B227" s="1" t="s">
+      <c r="B227" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C227" s="10">
@@ -6631,17 +6637,17 @@
         <v>178</v>
       </c>
       <c r="E227" s="17" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="F227" s="19">
         <v>218219</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A228" s="6" t="s">
+    <row r="228" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B228" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C228" s="10">
@@ -6651,17 +6657,17 @@
         <v>179</v>
       </c>
       <c r="E228" s="17" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F228" s="14">
         <v>214</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A229" s="6" t="s">
+    <row r="229" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B229" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C229" s="10">
@@ -6671,17 +6677,17 @@
         <v>180</v>
       </c>
       <c r="E229" s="17" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="F229" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A230" s="6" t="s">
+    <row r="230" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A230" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B230" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C230" s="10">
@@ -6691,7 +6697,7 @@
         <v>181</v>
       </c>
       <c r="E230" s="17" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="F230" s="14">
         <v>221</v>
@@ -6711,7 +6717,7 @@
         <v>183</v>
       </c>
       <c r="E231" s="17" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F231" s="14">
         <v>0</v>
@@ -6731,7 +6737,7 @@
         <v>184</v>
       </c>
       <c r="E232" s="17" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F232" s="14">
         <v>0</v>
@@ -6751,7 +6757,7 @@
         <v>185</v>
       </c>
       <c r="E233" s="17" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="F233" s="14">
         <v>0</v>
@@ -6771,7 +6777,7 @@
         <v>186</v>
       </c>
       <c r="E234" s="17" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F234" s="14">
         <v>0</v>
@@ -6791,7 +6797,7 @@
         <v>187</v>
       </c>
       <c r="E235" s="17" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F235" s="19">
         <v>231232</v>
@@ -6811,7 +6817,7 @@
         <v>188</v>
       </c>
       <c r="E236" s="17" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F236" s="14">
         <v>234</v>
@@ -6831,7 +6837,7 @@
         <v>189</v>
       </c>
       <c r="E237" s="17" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F237" s="14">
         <v>0</v>
@@ -6851,7 +6857,7 @@
         <v>190</v>
       </c>
       <c r="E238" s="17" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F238" s="14">
         <v>232</v>
@@ -6871,7 +6877,7 @@
         <v>191</v>
       </c>
       <c r="E239" s="17" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F239" s="14">
         <v>235</v>
@@ -6891,7 +6897,7 @@
         <v>192</v>
       </c>
       <c r="E240" s="17" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F240" s="14">
         <v>235</v>
@@ -6911,7 +6917,7 @@
         <v>193</v>
       </c>
       <c r="E241" s="17" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F241" s="14">
         <v>237</v>
@@ -6931,7 +6937,7 @@
         <v>194</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F242" s="14">
         <v>0</v>
@@ -6951,7 +6957,7 @@
         <v>195</v>
       </c>
       <c r="E243" s="16" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F243" s="19">
         <v>239240</v>
@@ -6971,7 +6977,7 @@
         <v>196</v>
       </c>
       <c r="E244" s="16" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F244" s="19">
         <v>239240</v>
@@ -6991,7 +6997,7 @@
         <v>197</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F245" s="14">
         <v>242</v>
@@ -7011,7 +7017,7 @@
         <v>198</v>
       </c>
       <c r="E246" s="16" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F246" s="19">
         <v>243244</v>
@@ -7031,7 +7037,7 @@
         <v>199</v>
       </c>
       <c r="E247" s="16" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F247" s="19">
         <v>243244</v>
@@ -7051,7 +7057,7 @@
         <v>200</v>
       </c>
       <c r="E248" s="16" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F248" s="19">
         <v>243244</v>
@@ -7071,7 +7077,7 @@
         <v>201</v>
       </c>
       <c r="E249" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F249" s="14">
         <v>245</v>

</xml_diff>